<commit_message>
0.22 change comparator in dds-channel
</commit_message>
<xml_diff>
--- a/Project Outputs for llrf_afe/BOM/llrf_afe.xlsx
+++ b/Project Outputs for llrf_afe/BOM/llrf_afe.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YandexDisk\Work\Altium\COSY\llrf_afe\Project Outputs for llrf_afe\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8E7F4A0-160D-46F6-8572-0516ED34C5A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E6A25C-CB60-4A33-848E-782A7B4158B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47640" yWindow="5715" windowWidth="28110" windowHeight="15885" xr2:uid="{E4E6C7E9-05EB-4740-9A7C-C746E8A3161B}"/>
+    <workbookView xWindow="4680" yWindow="4185" windowWidth="28110" windowHeight="15885" xr2:uid="{0258C881-A15B-4CE4-92F7-CD06B79E54C8}"/>
   </bookViews>
   <sheets>
     <sheet name="llrf_afe" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="290">
   <si>
     <t>Designator</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Конденсатор</t>
   </si>
   <si>
-    <t>SMD_0402</t>
+    <t>SMD_C0603</t>
   </si>
   <si>
     <t>NU</t>
@@ -81,7 +81,7 @@
     <t>90пФ</t>
   </si>
   <si>
-    <t>C7, C8, C9, C10, C16, C17, C18, C19, C23, C24, C30, C42, C43, C44, C45, C51, C52, C53, C54, C58, C59, C65, C77, C78, C79, C80, C86, C87, C88, C89, C93, C94, C100, C112, C113, C114, C115, C121, C122, C123, C124, C128, C129, C135, C141, C149, C154, C155, C156, C157, C158, C160, C162, C164, C165, C166, C173, C174, C194, C242, C243, C244, C245, C246, C259, C260, C262, C281, C283, C?_llrf_rio_ch1, C?_llrf_rio_ch2, C?_llrf_rio_ch3, C?_llrf_rio_ch4, C?_llrf_rio_ch5, C?_llrf_rio_ch6, C?_llrf_rio_ch7, C?_llrf_rio_ch8</t>
+    <t>C7, C8, C9, C16, C17, C18, C19, C23, C24, C30, C42, C43, C44, C51, C52, C53, C54, C58, C59, C65, C77, C78, C79, C86, C87, C88, C89, C93, C94, C100, C112, C113, C114, C121, C122, C123, C124, C128, C129, C135, C141, C149, C154, C155, C156, C157, C158, C160, C162, C164, C165, C166, C173, C174, C194, C242, C243, C244, C245, C246, C259, C260, C262, C264, C266, C268, C270, C272, C274, C276, C278, C281, C283</t>
   </si>
   <si>
     <t>SMD_C0402</t>
@@ -90,300 +90,288 @@
     <t>0.1мкФ</t>
   </si>
   <si>
-    <t>C11, C20, C21, C46, C55, C56, C81, C90, C91, C116, C125, C126</t>
+    <t>C11, C20, C21, C46, C55, C56, C81, C90, C91, C116, C125, C126, C143, C144, C145, C146, C167, C168, C169, C170</t>
   </si>
   <si>
     <t>GRM033D70J105ME01</t>
   </si>
   <si>
+    <t>1мкФ 6.3В X7T</t>
+  </si>
+  <si>
+    <t>C12, C14, C47, C49, C82, C84, C117, C119</t>
+  </si>
+  <si>
+    <t>62пФ</t>
+  </si>
+  <si>
+    <t>C22, C25, C26, C29, C31, C32, C35, C57, C60, C61, C64, C66, C67, C70, C92, C95, C96, C99, C101, C102, C105, C127, C130, C131, C134, C136, C137, C140, C172, C196, C198, C200, C202, C204, C217, C220, C221, C224, C226, C227, C229, C249, C252, C255, C258, C261, C263, C265, C267, C269, C271, C273, C275, C277</t>
+  </si>
+  <si>
+    <t>GRM188C81C106MA73</t>
+  </si>
+  <si>
+    <t>10мкФ 16В</t>
+  </si>
+  <si>
+    <t>C27, C28, C33, C34, C62, C63, C68, C69, C97, C98, C103, C104, C132, C133, C138, C139, C195, C197, C199, C201, C203, C205, C206, C208, C209, C210, C211, C216, C218, C219, C222, C223, C225, C228</t>
+  </si>
+  <si>
+    <t>C142</t>
+  </si>
+  <si>
+    <t>0.33мкФ</t>
+  </si>
+  <si>
+    <t>C147</t>
+  </si>
+  <si>
+    <t>1нФ</t>
+  </si>
+  <si>
+    <t>C148</t>
+  </si>
+  <si>
+    <t>0.3мкФ</t>
+  </si>
+  <si>
+    <t>C150, C151</t>
+  </si>
+  <si>
+    <t>0.47мкФ</t>
+  </si>
+  <si>
+    <t>C152, C153, C159, C161, C163, C171</t>
+  </si>
+  <si>
+    <t>3 Terminals Low ESL Chip Multilayer Ceramic Capacitors (EMIFIL) for General Purpose</t>
+  </si>
+  <si>
+    <t>NFM15PC105D0J3</t>
+  </si>
+  <si>
+    <t>3pol_SMD0402</t>
+  </si>
+  <si>
+    <t>1мкФ</t>
+  </si>
+  <si>
+    <t>C175, C176, C177, C178, C179, C180, C181, C182, C183, C184, C185, C186, C187, C188, C189, C190, C191, C192, C193</t>
+  </si>
+  <si>
+    <t>NFM15PC104D0J3</t>
+  </si>
+  <si>
+    <t>C207</t>
+  </si>
+  <si>
+    <t>100нФ</t>
+  </si>
+  <si>
+    <t>C212, C213, C214</t>
+  </si>
+  <si>
+    <t>33нФ</t>
+  </si>
+  <si>
+    <t>C215</t>
+  </si>
+  <si>
+    <t>SMD_C0805</t>
+  </si>
+  <si>
+    <t>47мкФ</t>
+  </si>
+  <si>
+    <t>C230</t>
+  </si>
+  <si>
+    <t>10мкФ</t>
+  </si>
+  <si>
+    <t>C231, C233, C236, C237, C238, C239, C240, C241</t>
+  </si>
+  <si>
+    <t>2.2мкФ</t>
+  </si>
+  <si>
+    <t>C232, C234, C235, C284, C285, C288</t>
+  </si>
+  <si>
+    <t>Поляризованный SMD-конденсатор</t>
+  </si>
+  <si>
+    <t>Поляризованный конденсатор</t>
+  </si>
+  <si>
+    <t>SMD_size_B</t>
+  </si>
+  <si>
+    <t>10мкФх50В</t>
+  </si>
+  <si>
+    <t>C247, C248, C250, C251, C253, C254, C256, C257</t>
+  </si>
+  <si>
+    <t>GRM033R61E224ME01</t>
+  </si>
+  <si>
+    <t>0.22мкФ 25В  X5R</t>
+  </si>
+  <si>
+    <t>C279, C280</t>
+  </si>
+  <si>
+    <t>47пФ</t>
+  </si>
+  <si>
+    <t>C282</t>
+  </si>
+  <si>
+    <t>10нФ</t>
+  </si>
+  <si>
+    <t>C286, C289</t>
+  </si>
+  <si>
+    <t>2.4нФ</t>
+  </si>
+  <si>
+    <t>C287, C290</t>
+  </si>
+  <si>
+    <t>16нФ</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>4 CHANNEL LOW CAPACITANCE TVS DIODE ARRAY</t>
+  </si>
+  <si>
+    <t>DRTR5V0U4S-7</t>
+  </si>
+  <si>
+    <t>SOT-363</t>
+  </si>
+  <si>
+    <t>D2, D3, D4, D5, D6</t>
+  </si>
+  <si>
+    <t>Светодиод</t>
+  </si>
+  <si>
+    <t>SMD-LED</t>
+  </si>
+  <si>
+    <t>LED-0805</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>D7, D8</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>G1</t>
+  </si>
+  <si>
+    <t>DC-DC преобразователь</t>
+  </si>
+  <si>
+    <t>TDN 5-0922WI</t>
+  </si>
+  <si>
+    <t>TDN_5_WISM</t>
+  </si>
+  <si>
+    <t>G2, G3, G4, G5</t>
+  </si>
+  <si>
+    <t>17-V Input 3-A Step-Down Converter MicroSiP™ Module with Integrated Inductor</t>
+  </si>
+  <si>
+    <t>TPS82130</t>
+  </si>
+  <si>
+    <t>uSiL-8</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>FMC HPC. Terminal Array Assembly, Surface Mount, 0.050" Pitch, 400 Pins</t>
+  </si>
+  <si>
+    <t>ASP-134486-01</t>
+  </si>
+  <si>
+    <t>L1, L2, L11, L12, L21, L22, L31, L32</t>
+  </si>
+  <si>
+    <t>SMD-индуктивность</t>
+  </si>
+  <si>
+    <t>Индуктивность</t>
+  </si>
+  <si>
+    <t>SMD_0805</t>
+  </si>
+  <si>
+    <t>50нГн</t>
+  </si>
+  <si>
+    <t>L3, L4, L13, L14, L23, L24, L33, L34</t>
+  </si>
+  <si>
+    <t>110нГн</t>
+  </si>
+  <si>
+    <t>L5, L15, L25, L35</t>
+  </si>
+  <si>
+    <t>200нГн</t>
+  </si>
+  <si>
+    <t>L6, L16, L26, L36</t>
+  </si>
+  <si>
+    <t>130нГн</t>
+  </si>
+  <si>
+    <t>L7, L8, L9, L10, L17, L18, L19, L20, L27, L28, L29, L30, L37, L38, L39, L40, L41, L42, L43, L44, L45, L46, L48, L49, L50, L51, L52</t>
+  </si>
+  <si>
+    <t>1мкГн</t>
+  </si>
+  <si>
+    <t>L47</t>
+  </si>
+  <si>
+    <t>SDR0805-221KL</t>
+  </si>
+  <si>
+    <t>SDR0805</t>
+  </si>
+  <si>
+    <t>220мкГн</t>
+  </si>
+  <si>
+    <t>R1, R16, R24, R39, R47, R62, R70, R85, R94, R95, R99, R100, R117, R139, R140, R141, R145, R146, R147, R151, R152, R153, R157, R158, R159, R163, R164, R165, R183, R190</t>
+  </si>
+  <si>
+    <t>SMD-резистор</t>
+  </si>
+  <si>
+    <t>Резистор</t>
+  </si>
+  <si>
     <t>SMD_0603</t>
   </si>
   <si>
-    <t>1мкФ 6.3В X7T</t>
-  </si>
-  <si>
-    <t>C12, C14, C47, C49, C82, C84, C117, C119</t>
-  </si>
-  <si>
-    <t>62пФ</t>
-  </si>
-  <si>
-    <t>C22, C25, C26, C29, C32, C35, C57, C60, C61, C64, C67, C70, C92, C95, C96, C99, C102, C105, C127, C130, C131, C134, C137, C140</t>
-  </si>
-  <si>
-    <t>GRM188C81C106MA73</t>
-  </si>
-  <si>
-    <t>10мкФ 16В</t>
-  </si>
-  <si>
-    <t>C27, C28, C33, C34, C62, C63, C68, C69, C97, C98, C103, C104, C132, C133, C138, C139, C195, C201, C202, C203, C204, C205, C206, C208, C209, C210, C211, C216, C218, C219, C222, C223, C225, C227</t>
-  </si>
-  <si>
-    <t>SMD_C0603</t>
-  </si>
-  <si>
-    <t>C31, C66, C101, C136, C172, C196, C197, C198, C199, C200, C217, C220, C221, C224, C228, C249, C252, C255, C258, C261, C?, C?_llrf_rio_ch1, C?_llrf_rio_ch2, C?_llrf_rio_ch3, C?_llrf_rio_ch4, C?_llrf_rio_ch5, C?_llrf_rio_ch6, C?_llrf_rio_ch7, C?_llrf_rio_ch8</t>
-  </si>
-  <si>
-    <t>C142</t>
-  </si>
-  <si>
-    <t>0.33мкФ</t>
-  </si>
-  <si>
-    <t>C143, C144, C145, C146, C167, C168, C169, C170</t>
-  </si>
-  <si>
-    <t>C147</t>
-  </si>
-  <si>
-    <t>1нФ</t>
-  </si>
-  <si>
-    <t>C148</t>
-  </si>
-  <si>
-    <t>0.3мкФ</t>
-  </si>
-  <si>
-    <t>C150, C151</t>
-  </si>
-  <si>
-    <t>0.47мкФ</t>
-  </si>
-  <si>
-    <t>C152, C153, C159, C161, C163, C171</t>
-  </si>
-  <si>
-    <t>3 Terminals Low ESL Chip Multilayer Ceramic Capacitors (EMIFIL) for General Purpose</t>
-  </si>
-  <si>
-    <t>NFM15PC105D0J3</t>
-  </si>
-  <si>
-    <t>3pol_SMD0402</t>
-  </si>
-  <si>
-    <t>1мкФ</t>
-  </si>
-  <si>
-    <t>C175, C176, C177, C178, C179, C180, C181, C182, C183, C184, C185, C186, C187, C188, C189, C190, C191, C192, C193</t>
-  </si>
-  <si>
-    <t>NFM15PC104D0J3</t>
-  </si>
-  <si>
-    <t>C207</t>
-  </si>
-  <si>
-    <t>100нФ</t>
-  </si>
-  <si>
-    <t>C212, C213, C214</t>
-  </si>
-  <si>
-    <t>33нФ</t>
-  </si>
-  <si>
-    <t>C215</t>
-  </si>
-  <si>
-    <t>SMD_C0805</t>
-  </si>
-  <si>
-    <t>47мкФ</t>
-  </si>
-  <si>
-    <t>C229</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>10мкФ</t>
-  </si>
-  <si>
-    <t>C231, C233, C236, C237, C238, C239, C240, C241</t>
-  </si>
-  <si>
-    <t>2.2мкФ</t>
-  </si>
-  <si>
-    <t>C232, C234, C235, C284, C285, C288</t>
-  </si>
-  <si>
-    <t>Поляризованный SMD-конденсатор</t>
-  </si>
-  <si>
-    <t>Поляризованный конденсатор</t>
-  </si>
-  <si>
-    <t>SMD_size_B</t>
-  </si>
-  <si>
-    <t>10мкФх50В</t>
-  </si>
-  <si>
-    <t>C247, C248, C250, C251, C253, C254, C256, C257</t>
-  </si>
-  <si>
-    <t>GRM033R61E224ME01</t>
-  </si>
-  <si>
-    <t>0.22мкФ 25В  X5R</t>
-  </si>
-  <si>
-    <t>C279, C280</t>
-  </si>
-  <si>
-    <t>47пФ</t>
-  </si>
-  <si>
-    <t>C282</t>
-  </si>
-  <si>
-    <t>10нФ</t>
-  </si>
-  <si>
-    <t>C286, C289</t>
-  </si>
-  <si>
-    <t>2.4нФ</t>
-  </si>
-  <si>
-    <t>C287, C290</t>
-  </si>
-  <si>
-    <t>16нФ</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>4 CHANNEL LOW CAPACITANCE TVS DIODE ARRAY</t>
-  </si>
-  <si>
-    <t>DRTR5V0U4S-7</t>
-  </si>
-  <si>
-    <t>SOT-363</t>
-  </si>
-  <si>
-    <t>D2, D3, D4, D5, D6</t>
-  </si>
-  <si>
-    <t>Светодиод</t>
-  </si>
-  <si>
-    <t>SMD-LED</t>
-  </si>
-  <si>
-    <t>LED-0805</t>
-  </si>
-  <si>
-    <t>green</t>
-  </si>
-  <si>
-    <t>D7, D8</t>
-  </si>
-  <si>
-    <t>RED</t>
-  </si>
-  <si>
-    <t>G1</t>
-  </si>
-  <si>
-    <t>DC-DC преобразователь</t>
-  </si>
-  <si>
-    <t>TDN 5-0922WI</t>
-  </si>
-  <si>
-    <t>TDN_5_WISM</t>
-  </si>
-  <si>
-    <t>G2, G3, G4, G5</t>
-  </si>
-  <si>
-    <t>17-V Input 3-A Step-Down Converter MicroSiP™ Module with Integrated Inductor</t>
-  </si>
-  <si>
-    <t>TPS82130</t>
-  </si>
-  <si>
-    <t>uSiL-8</t>
-  </si>
-  <si>
-    <t>J1</t>
-  </si>
-  <si>
-    <t>FMC HPC. Terminal Array Assembly, Surface Mount, 0.050" Pitch, 400 Pins</t>
-  </si>
-  <si>
-    <t>ASP-134486-01</t>
-  </si>
-  <si>
-    <t>L1, L2, L11, L12, L21, L22, L31, L32</t>
-  </si>
-  <si>
-    <t>SMD-индуктивность</t>
-  </si>
-  <si>
-    <t>Индуктивность</t>
-  </si>
-  <si>
-    <t>SMD_0805</t>
-  </si>
-  <si>
-    <t>50нГн</t>
-  </si>
-  <si>
-    <t>L3, L4, L13, L14, L23, L24, L33, L34</t>
-  </si>
-  <si>
-    <t>110нГн</t>
-  </si>
-  <si>
-    <t>L5, L15, L25, L35</t>
-  </si>
-  <si>
-    <t>200нГн</t>
-  </si>
-  <si>
-    <t>L6, L16, L26, L36</t>
-  </si>
-  <si>
-    <t>130нГн</t>
-  </si>
-  <si>
-    <t>L7, L8, L9, L10, L17, L18, L19, L20, L27, L28, L29, L30, L37, L38, L39, L40, L41, L42, L43, L44, L45, L46, L48, L49, L50, L51, L52</t>
-  </si>
-  <si>
-    <t>1мкГн</t>
-  </si>
-  <si>
-    <t>L47</t>
-  </si>
-  <si>
-    <t>SDR0805-221KL</t>
-  </si>
-  <si>
-    <t>SDR0805</t>
-  </si>
-  <si>
-    <t>220мкГн</t>
-  </si>
-  <si>
-    <t>R1, R16, R24, R39, R47, R62, R70, R85, R94, R95, R99, R100, R117, R139, R140, R141, R145, R146, R147, R151, R152, R153, R157, R158, R159, R163, R164, R165, R183, R190</t>
-  </si>
-  <si>
-    <t>SMD-резистор</t>
-  </si>
-  <si>
-    <t>Резистор</t>
-  </si>
-  <si>
     <t>100</t>
   </si>
   <si>
@@ -393,7 +381,7 @@
     <t>49.9</t>
   </si>
   <si>
-    <t>R3, R7, R26, R30, R49, R53, R72, R76, R101, R102, R103, R104, R105, R122, R123, R124, R126, R127, R133, R137, R143, R149, R155, R161, R182, R184, R185, R189, R191, R192, R288, R297</t>
+    <t>R3, R7, R13, R26, R30, R36, R49, R53, R59, R72, R76, R82, R101, R102, R103, R104, R105, R122, R123, R124, R126, R127, R133, R137, R143, R149, R155, R161, R182, R184, R185, R189, R191, R192, R288, R297</t>
   </si>
   <si>
     <t>10к</t>
@@ -414,9 +402,6 @@
     <t>1к</t>
   </si>
   <si>
-    <t>R13, R36, R59, R82</t>
-  </si>
-  <si>
     <t>R20, R21, R43, R44, R66, R67, R89, R90, R212, R213, R221, R222, R230, R231, R239, R240, R248, R249, R257, R258, R266, R267, R275, R276</t>
   </si>
   <si>
@@ -582,18 +567,6 @@
     <t>ADT1-6T</t>
   </si>
   <si>
-    <t>TP1</t>
-  </si>
-  <si>
-    <t>Контроль параметров платы</t>
-  </si>
-  <si>
-    <t>Точка проверки</t>
-  </si>
-  <si>
-    <t>TestPoint</t>
-  </si>
-  <si>
     <t>U1, U5, U9, U13</t>
   </si>
   <si>
@@ -819,7 +792,7 @@
     <t>SOT-23</t>
   </si>
   <si>
-    <t>X1, X3, X4, X5, X7, X8, X9, X11, X12, X13, X15, X16, X22, X23, X30, X31, X32, X33, X34, X35, X36, X37</t>
+    <t>X1, X3, X4, X5, X7, X8, X9, X11, X12, X13, X15, X16, X22, X23, X31, X32, X33, X34, X35, X36, X37, X38</t>
   </si>
   <si>
     <t>Jumper, 3-Pin, Dual row</t>
@@ -831,7 +804,7 @@
     <t>PLS-3</t>
   </si>
   <si>
-    <t>X2, X6, X10, X14, X29</t>
+    <t>X2, X6, X10, X14, X30</t>
   </si>
   <si>
     <t>Jumper, 2-Pin, Dual row</t>
@@ -843,7 +816,7 @@
     <t>PLS-2</t>
   </si>
   <si>
-    <t>X17, X18, X19, X20, X24, X25, X26</t>
+    <t>X17, X18, X19, X20, X24, X25, X27</t>
   </si>
   <si>
     <t xml:space="preserve">LEMO Connector, coax 1-pin </t>
@@ -861,7 +834,16 @@
     <t>EPG.0B.302.HLN</t>
   </si>
   <si>
-    <t>X27</t>
+    <t>X26</t>
+  </si>
+  <si>
+    <t>Header, 20-Pin, Dual row</t>
+  </si>
+  <si>
+    <t>PLD2-20</t>
+  </si>
+  <si>
+    <t>X28</t>
   </si>
   <si>
     <t>BH-10R (DS1013-10R) (IDC-10MR), Вилка на плату угловая 10 конт. 2.54мм</t>
@@ -870,7 +852,7 @@
     <t>DS1013-10R</t>
   </si>
   <si>
-    <t>X28</t>
+    <t>X29</t>
   </si>
   <si>
     <t>Вилка на плату угловая 4.2мм 8pin со втулками</t>
@@ -882,7 +864,7 @@
     <t>KLS1-4.20-2X04</t>
   </si>
   <si>
-    <t>X38</t>
+    <t>X39</t>
   </si>
   <si>
     <t>MicroUSB bottom mount receptacle, B-type</t>
@@ -892,15 +874,6 @@
   </si>
   <si>
     <t>MicroUSB-Molex-105017</t>
-  </si>
-  <si>
-    <t>X39</t>
-  </si>
-  <si>
-    <t>Header, 20-Pin, Dual row</t>
-  </si>
-  <si>
-    <t>PLD2-20</t>
   </si>
   <si>
     <t>Y1</t>
@@ -1301,10 +1274,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5EB5A39-5844-47D8-A2BF-EC1BDF84BD40}">
-  <dimension ref="A1:F107"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{486C07AB-40AD-41B6-923F-9F36A9AABE00}">
+  <dimension ref="A1:F103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A95" sqref="A95"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1430,7 +1405,7 @@
         <v>18</v>
       </c>
       <c r="E6" s="1">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>19</v>
@@ -1447,18 +1422,18 @@
         <v>21</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="1">
+        <v>20</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="E7" s="1">
-        <v>12</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>7</v>
@@ -1473,32 +1448,32 @@
         <v>8</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="1">
+        <v>54</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="1">
-        <v>24</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>7</v>
@@ -1507,7 +1482,7 @@
         <v>8</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="E10" s="1">
         <v>34</v>
@@ -1518,27 +1493,27 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="E11" s="1">
-        <v>30</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>7</v>
@@ -1553,27 +1528,27 @@
         <v>1</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="E13" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1590,7 +1565,7 @@
         <v>18</v>
       </c>
       <c r="E14" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>36</v>
@@ -1601,56 +1576,56 @@
         <v>37</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="E15" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="E16" s="1">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="E17" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>45</v>
@@ -1661,19 +1636,19 @@
         <v>46</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="1">
+        <v>3</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" s="1">
-        <v>19</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1687,18 +1662,18 @@
         <v>8</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="E19" s="1">
         <v>1</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>7</v>
@@ -1707,18 +1682,18 @@
         <v>8</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="E20" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>7</v>
@@ -1727,10 +1702,10 @@
         <v>8</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="E21" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>54</v>
@@ -1741,56 +1716,56 @@
         <v>55</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E22" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="E23" s="1">
         <v>8</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>61</v>
+        <v>7</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>62</v>
+        <v>8</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="E24" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>64</v>
@@ -1804,21 +1779,21 @@
         <v>7</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E25" s="1">
-        <v>8</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>7</v>
@@ -1833,12 +1808,12 @@
         <v>2</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>7</v>
@@ -1850,122 +1825,118 @@
         <v>18</v>
       </c>
       <c r="E27" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="C28" s="2" t="s">
-        <v>8</v>
+        <v>73</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="E28" s="1">
-        <v>2</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>73</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>7</v>
+        <v>76</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>8</v>
+        <v>77</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="E29" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="E30" s="1">
-        <v>1</v>
-      </c>
-      <c r="F30" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E31" s="1">
-        <v>5</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>84</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="E32" s="1">
-        <v>2</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>86</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E33" s="1">
         <v>1</v>
@@ -1974,146 +1945,150 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E34" s="1">
-        <v>4</v>
-      </c>
-      <c r="F34" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>97</v>
-      </c>
       <c r="E35" s="1">
-        <v>1</v>
-      </c>
-      <c r="F35" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D36" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E36" s="1">
+        <v>4</v>
+      </c>
+      <c r="F36" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="E36" s="1">
-        <v>8</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E37" s="1">
+        <v>4</v>
+      </c>
+      <c r="F37" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E37" s="1">
-        <v>8</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E38" s="1">
+        <v>27</v>
+      </c>
+      <c r="F38" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E38" s="1">
-        <v>4</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>100</v>
-      </c>
       <c r="D39" s="2" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="E39" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="E40" s="1">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>112</v>
@@ -2122,27 +2097,27 @@
         <v>113</v>
       </c>
       <c r="E41" s="1">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>22</v>
+        <v>113</v>
       </c>
       <c r="E42" s="1">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>118</v>
@@ -2153,16 +2128,16 @@
         <v>119</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>22</v>
+        <v>113</v>
       </c>
       <c r="E43" s="1">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>120</v>
@@ -2173,179 +2148,179 @@
         <v>121</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>22</v>
+        <v>113</v>
       </c>
       <c r="E44" s="1">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>122</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E45" s="1">
+        <v>24</v>
+      </c>
+      <c r="F45" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E45" s="1">
-        <v>38</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="E46" s="1">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>10</v>
+        <v>126</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>22</v>
+        <v>113</v>
       </c>
       <c r="E47" s="1">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>9</v>
+        <v>113</v>
       </c>
       <c r="E48" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="E49" s="1">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>22</v>
+        <v>113</v>
       </c>
       <c r="E50" s="1">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>22</v>
+        <v>113</v>
       </c>
       <c r="E51" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="E52" s="1">
         <v>1</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -2353,16 +2328,16 @@
         <v>138</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>22</v>
+        <v>113</v>
       </c>
       <c r="E53" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>139</v>
@@ -2373,16 +2348,16 @@
         <v>140</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>22</v>
+        <v>113</v>
       </c>
       <c r="E54" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>141</v>
@@ -2393,179 +2368,179 @@
         <v>142</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>22</v>
+        <v>113</v>
       </c>
       <c r="E55" s="1">
         <v>1</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>22</v>
+        <v>113</v>
       </c>
       <c r="E56" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>22</v>
+        <v>113</v>
       </c>
       <c r="E57" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>22</v>
+        <v>113</v>
       </c>
       <c r="E58" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>22</v>
+        <v>113</v>
       </c>
       <c r="E59" s="1">
         <v>1</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>117</v>
+        <v>153</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>22</v>
+        <v>125</v>
       </c>
       <c r="E60" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>22</v>
+        <v>113</v>
       </c>
       <c r="E61" s="1">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>22</v>
+        <v>113</v>
       </c>
       <c r="E62" s="1">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E63" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>159</v>
+        <v>139</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -2573,79 +2548,79 @@
         <v>160</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>117</v>
+        <v>153</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>22</v>
+        <v>125</v>
       </c>
       <c r="E64" s="1">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>117</v>
+        <v>153</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>22</v>
+        <v>125</v>
       </c>
       <c r="E65" s="1">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>163</v>
+        <v>118</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>158</v>
+        <v>112</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="E66" s="1">
         <v>2</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>144</v>
+        <v>163</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E67" s="1">
+        <v>5</v>
+      </c>
+      <c r="F67" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E67" s="1">
-        <v>1</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -2653,173 +2628,167 @@
         <v>166</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>158</v>
+        <v>112</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="E68" s="1">
         <v>1</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>122</v>
+        <v>167</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>22</v>
+        <v>113</v>
       </c>
       <c r="E69" s="1">
         <v>2</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>22</v>
+        <v>113</v>
       </c>
       <c r="E70" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>22</v>
+        <v>113</v>
       </c>
       <c r="E71" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>22</v>
+        <v>113</v>
       </c>
       <c r="E72" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>116</v>
+        <v>177</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>117</v>
+        <v>178</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>22</v>
+        <v>178</v>
       </c>
       <c r="E73" s="1">
-        <v>1</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>176</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="F73" s="1"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>116</v>
+        <v>180</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>117</v>
+        <v>181</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>22</v>
+        <v>182</v>
       </c>
       <c r="E74" s="1">
-        <v>2</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>178</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="F74" s="1"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>116</v>
+        <v>184</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>117</v>
+        <v>185</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>22</v>
+        <v>186</v>
       </c>
       <c r="E75" s="1">
-        <v>1</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>180</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F75" s="1"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="E76" s="1">
         <v>4</v>
@@ -2828,106 +2797,106 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="E77" s="1">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="F77" s="1"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="E78" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F78" s="1"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="E79" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F79" s="1"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="E80" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F80" s="1"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="E81" s="1">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="F81" s="1"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="E82" s="1">
         <v>1</v>
@@ -2936,16 +2905,16 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="E83" s="1">
         <v>1</v>
@@ -2954,16 +2923,16 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="E84" s="1">
         <v>1</v>
@@ -2972,106 +2941,106 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="E85" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F85" s="1"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="E86" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F86" s="1"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="E87" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F87" s="1"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="E88" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F88" s="1"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="E89" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F89" s="1"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>233</v>
+        <v>243</v>
       </c>
       <c r="E90" s="1">
         <v>2</v>
@@ -3080,196 +3049,196 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="E91" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F91" s="1"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="E92" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F92" s="1"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="E93" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F93" s="1"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="E94" s="1">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="F94" s="1"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="E95" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F95" s="1"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c r="E96" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F96" s="1"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="E97" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F97" s="1"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="E98" s="1">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="F98" s="1"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="E99" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F99" s="1"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="E100" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F100" s="1"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="E101" s="1">
         <v>1</v>
@@ -3278,16 +3247,16 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="E102" s="1">
         <v>1</v>
@@ -3296,93 +3265,21 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="E103" s="1">
         <v>1</v>
       </c>
       <c r="F103" s="1"/>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="D104" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="E104" s="1">
-        <v>1</v>
-      </c>
-      <c r="F104" s="1"/>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="D105" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="E105" s="1">
-        <v>1</v>
-      </c>
-      <c r="F105" s="1"/>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="C106" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="D106" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="E106" s="1">
-        <v>1</v>
-      </c>
-      <c r="F106" s="1"/>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="D107" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="E107" s="1">
-        <v>1</v>
-      </c>
-      <c r="F107" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
0.50 fix FPAG configuration memory
</commit_message>
<xml_diff>
--- a/Project Outputs for llrf_afe/BOM/llrf_afe.xlsx
+++ b/Project Outputs for llrf_afe/BOM/llrf_afe.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YandexDisk\Work\Altium\COSY\llrf_afe\Project Outputs for llrf_afe\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{94B6190B-6CC6-4FA2-A112-A4D85EACBE71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3B685A-6707-4297-9740-A2090BDED083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44460" yWindow="5625" windowWidth="28110" windowHeight="15885" xr2:uid="{0D76ABD2-A188-40C2-83CE-914084438B79}"/>
+    <workbookView xWindow="13755" yWindow="2835" windowWidth="28110" windowHeight="15885" xr2:uid="{C09BF35C-D0E0-45A9-B6AD-F4DB426FEBD2}"/>
   </bookViews>
   <sheets>
     <sheet name="llrf_afe" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,19 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="328">
   <si>
     <t>Designator</t>
   </si>
@@ -48,7 +55,7 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>C1, C8, C9, C10, C11, C16, C17, C18, C19, C20, C22, C24, C26, C27, C28, C54, C56, C57, C58, C59, C60, C62, C63, C64, C65, C83, C84, C86, C88, C90, C94, C95, C97, C98, C99, C100, C105, C107, C108, C111, C112, C114, C117, C131, C132, C133, C134, C135, C148, C149, C151, C153, C155, C157, C159, C161, C163, C165, C167, C170, C172, C180, C181, C182, C183, C184, C186, C187, C190, C191, C194, C196, C197, C198, C200, C201, C202, C203, C204, C212, C218, C221, C222, C229, C235, C238, C239, C240, C241, C242, C244, C245, C248, C249, C252, C254, C255, C256, C258, C259, C260, C261, C262, C270, C276, C279, C280, C287, C293, C296, C297</t>
+    <t>C1, C8, C9, C10, C11, C16, C17, C18, C19, C20, C22, C24, C26, C27, C28, C52, C54, C55, C56, C57, C58, C60, C61, C62, C63, C82, C83, C85, C87, C89, C91, C92, C94, C95, C96, C97, C102, C104, C105, C108, C109, C111, C114, C128, C129, C130, C131, C132, C145, C146, C148, C150, C152, C154, C156, C158, C160, C162, C164, C167, C169, C177, C178, C179, C180, C181, C183, C184, C187, C188, C191, C193, C194, C195, C196, C197, C198, C199, C200, C208, C214, C217, C218, C225, C231, C234, C235, C236, C237, C238, C240, C241, C244, C245, C248, C250, C251, C252, C253, C254, C255, C256, C257, C265, C271, C274, C275, C282, C288, C291, C292</t>
   </si>
   <si>
     <t>SMD-конденсатор</t>
@@ -69,7 +76,7 @@
     <t>0.33мкФ</t>
   </si>
   <si>
-    <t>C3, C4, C5, C6, C29, C30, C31, C32, C213, C219, C220, C230, C236, C237, C271, C277, C278, C288, C294, C295</t>
+    <t>C3, C4, C5, C6, C29, C30, C31, C32, C209, C215, C216, C226, C232, C233, C266, C272, C273, C283, C289, C290</t>
   </si>
   <si>
     <t>GRM033D70J105ME01</t>
@@ -81,7 +88,7 @@
     <t>SMD_C0603</t>
   </si>
   <si>
-    <t>C7, C205, C263</t>
+    <t>C7, C201, C258</t>
   </si>
   <si>
     <t>1нФ</t>
@@ -93,7 +100,7 @@
     <t>0.47мкФ</t>
   </si>
   <si>
-    <t>C14, C15, C21, C23, C25, C52, C53</t>
+    <t>C14, C15, C21, C23, C25, C50, C51</t>
   </si>
   <si>
     <t>3 Terminals Low ESL Chip Multilayer Ceramic Capacitors (EMIFIL) for General Purpose</t>
@@ -108,13 +115,13 @@
     <t>3pol_SMD0402</t>
   </si>
   <si>
-    <t>C33, C34, C35, C36, C37, C38, C39, C40, C41, C42, C43, C44, C45, C46, C47, C48, C49, C50, C51, C66, C67, C68, C69, C70, C71, C72, C73, C74</t>
+    <t>C33, C34, C35, C36, C37, C38, C39, C40, C41, C42, C43, C44, C45, C46, C47, C48, C49, C64, C65, C66, C67, C68, C69, C70, C71, C72, C73</t>
   </si>
   <si>
     <t>NFM15PC104D0J3</t>
   </si>
   <si>
-    <t>C55, C61</t>
+    <t>C53, C59</t>
   </si>
   <si>
     <t>Поляризованный SMD-конденсатор</t>
@@ -129,7 +136,7 @@
     <t>SMD_size_B</t>
   </si>
   <si>
-    <t>C75, C76, C77, C78, C79, C80, C81, C82</t>
+    <t>C74, C75, C76, C77, C78, C79, C80, C81</t>
   </si>
   <si>
     <t>1нФ 2кВ</t>
@@ -138,117 +145,114 @@
     <t>SMD_C1206</t>
   </si>
   <si>
-    <t>C85, C87, C89, C91, C106, C109, C110, C113, C115, C116, C118, C138, C141, C144, C147, C150, C152, C154, C156, C158, C160, C162, C164, C166, C185, C188, C189, C192, C193, C195, C243, C246, C247, C250, C251, C253</t>
+    <t>C84, C86, C88, C90, C103, C106, C107, C110, C112, C113, C115, C116</t>
+  </si>
+  <si>
+    <t>10мкФ 16В</t>
+  </si>
+  <si>
+    <t>C93</t>
+  </si>
+  <si>
+    <t>C98, C99, C100</t>
+  </si>
+  <si>
+    <t>33нФ</t>
+  </si>
+  <si>
+    <t>C101</t>
+  </si>
+  <si>
+    <t>47мкФ</t>
+  </si>
+  <si>
+    <t>SMD_C0805</t>
+  </si>
+  <si>
+    <t>C117, C119, C122, C123, C124, C125, C126, C127</t>
+  </si>
+  <si>
+    <t>2.2мкФ</t>
+  </si>
+  <si>
+    <t>C118, C120, C121, C170, C171, C174</t>
+  </si>
+  <si>
+    <t>10мкФх50В</t>
+  </si>
+  <si>
+    <t>C133, C134, C136, C137, C139, C140, C142, C143</t>
+  </si>
+  <si>
+    <t>0.22мкФ 25В X7R</t>
+  </si>
+  <si>
+    <t>C135, C138, C141, C144, C147, C149, C151, C153, C155, C157, C159, C161, C163, C182, C185, C186, C189, C190, C192, C239, C242, C243, C246, C247, C249</t>
   </si>
   <si>
     <t>GRM188C81C106MA73</t>
   </si>
   <si>
-    <t>10мкФ 16В</t>
-  </si>
-  <si>
-    <t>C96</t>
-  </si>
-  <si>
-    <t>100нФ</t>
-  </si>
-  <si>
-    <t>C101, C102, C103</t>
-  </si>
-  <si>
-    <t>33нФ</t>
-  </si>
-  <si>
-    <t>C104</t>
-  </si>
-  <si>
-    <t>47мкФ</t>
-  </si>
-  <si>
-    <t>SMD_C0805</t>
-  </si>
-  <si>
-    <t>C119</t>
-  </si>
-  <si>
-    <t>10мкФ</t>
-  </si>
-  <si>
-    <t>C120, C122, C125, C126, C127, C128, C129, C130</t>
-  </si>
-  <si>
-    <t>2.2мкФ</t>
-  </si>
-  <si>
-    <t>C121, C123, C124, C173, C174, C177</t>
-  </si>
-  <si>
-    <t>10мкФх50В</t>
-  </si>
-  <si>
-    <t>C136, C137, C139, C140, C142, C143, C145, C146</t>
-  </si>
-  <si>
-    <t>GRM033R61E224ME01</t>
-  </si>
-  <si>
-    <t>0.22мкФ 25В  X5R</t>
-  </si>
-  <si>
-    <t>C168, C169</t>
+    <t>C165, C166</t>
   </si>
   <si>
     <t>47пФ</t>
   </si>
   <si>
-    <t>C171</t>
+    <t>C168</t>
   </si>
   <si>
     <t>10нФ</t>
   </si>
   <si>
-    <t>C175, C178</t>
+    <t>C172, C175</t>
   </si>
   <si>
     <t>2.4нФ</t>
   </si>
   <si>
-    <t>C176, C179</t>
+    <t>C173, C176</t>
   </si>
   <si>
     <t>16нФ</t>
   </si>
   <si>
-    <t>C206, C215, C217, C223, C232, C234, C264, C273, C275, C281, C290, C292</t>
+    <t>C202, C211, C213, C219, C228, C230, C259, C268, C270, C276, C285, C287</t>
   </si>
   <si>
     <t>NU</t>
   </si>
   <si>
-    <t>C207, C224, C265, C282</t>
+    <t>C203, C220, C260, C277</t>
   </si>
   <si>
     <t>13пФ</t>
   </si>
   <si>
-    <t>C208, C209, C225, C226, C266, C267, C283, C284</t>
+    <t>C204, C205, C221, C222, C261, C262, C278, C279</t>
   </si>
   <si>
     <t>32пФ</t>
   </si>
   <si>
-    <t>C210, C211, C227, C228, C268, C269, C285, C286</t>
+    <t>C206, C207, C223, C224, C263, C264, C280, C281</t>
   </si>
   <si>
     <t>91пФ</t>
   </si>
   <si>
-    <t>C214, C216, C231, C233, C272, C274, C289, C291</t>
+    <t>C210, C212, C227, C229, C267, C269, C284, C286</t>
   </si>
   <si>
     <t>62пФ</t>
   </si>
   <si>
+    <t>C293, C294, C295, C296</t>
+  </si>
+  <si>
+    <t>10мкФ 16В X7R</t>
+  </si>
+  <si>
     <t>D1, D2, D3, D4, D5</t>
   </si>
   <si>
@@ -282,6 +286,18 @@
     <t>SOT-363</t>
   </si>
   <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>Circuit Board Indicator</t>
+  </si>
+  <si>
+    <t>WP130WCP/2EGW</t>
+  </si>
+  <si>
+    <t>WP130WCP</t>
+  </si>
+  <si>
     <t>G1</t>
   </si>
   <si>
@@ -366,7 +382,7 @@
     <t>130нГн</t>
   </si>
   <si>
-    <t>R1, R4, R5, R6, R29, R36, R41, R194, R206, R235, R238, R241, R242, R244, R262, R265, R268, R269, R271, R307, R310, R313, R314, R316, R334, R337, R340, R341, R343</t>
+    <t>R1, R4, R5, R6, R33, R40, R45, R198, R211, R241, R244, R247, R248, R250, R268, R271, R274, R275, R277, R314, R317, R320, R321, R323, R341, R344, R347, R348, R350</t>
   </si>
   <si>
     <t>SMD-резистор</t>
@@ -381,19 +397,46 @@
     <t>SMD_0603</t>
   </si>
   <si>
-    <t>R2, R3, R7, R8, R9, R10, R11, R12, R13, R14, R15, R17, R18, R19, R20, R21, R22, R24, R40, R64, R65, R66, R72, R73, R74, R80, R81, R82, R88, R89, R90, R96, R97, R98, R116, R123, R230, R257, R302, R329</t>
+    <t>R2, R3, R8, R10, R12, R14, R15, R16, R17, R18, R19, R21, R22, R23, R25, R28, R44, R68, R69, R70, R76, R77, R78, R84, R85, R86, R92, R93, R94, R100, R101, R102, R120, R127, R236, R263, R309, R336</t>
   </si>
   <si>
     <t>100</t>
   </si>
   <si>
-    <t>R16, R126, R128, R130, R140, R146, R152, R158, R164, R170, R176, R182</t>
+    <t>R7, R9, R11, R13, R208</t>
+  </si>
+  <si>
+    <t>4 Chip Resistor Array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC124-FR-0733RL </t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>TC124</t>
+  </si>
+  <si>
+    <t>R20, R130, R132, R134, R144, R150, R156, R162, R168, R174, R180, R186</t>
   </si>
   <si>
     <t>200</t>
   </si>
   <si>
-    <t>R23</t>
+    <t>R24</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>R26, R115, R116, R117</t>
+  </si>
+  <si>
+    <t>240</t>
+  </si>
+  <si>
+    <t>R27</t>
   </si>
   <si>
     <t>1M</t>
@@ -402,160 +445,145 @@
     <t>SMD_1206</t>
   </si>
   <si>
-    <t>R25, R38, R39, R183, R184</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>R26, R27, R28, R45, R46, R47, R49, R50, R56, R60, R68, R76, R84, R92, R115, R117, R118, R122, R124, R125, R186, R190, R199, R204, R205, R207, R208, R209, R210, R211, R214, R215, R218, R219, R222, R223, R224, R225, R226, R227, R239, R248, R249, R251, R253, R266, R275, R276, R278, R280, R286, R287, R290, R291, R294, R295, R296, R297, R298, R299, R311, R320, R321, R323, R325, R338, R347, R348, R350, R352, R357, R358</t>
+    <t>R29, R42, R43, R187, R188, R207</t>
+  </si>
+  <si>
+    <t>R30, R31, R32, R49, R50, R51, R53, R54, R60, R64, R72, R80, R88, R96, R119, R121, R122, R126, R128, R129, R190, R194, R203, R209, R210, R212, R213, R214, R215, R216, R219, R220, R223, R224, R227, R228, R229, R230, R231, R232, R233, R245, R254, R255, R257, R259, R272, R281, R282, R284, R286, R292, R293, R296, R297, R300, R301, R302, R303, R304, R305, R306, R318, R327, R328, R330, R332, R345, R354, R355, R357, R359</t>
   </si>
   <si>
     <t>10к</t>
   </si>
   <si>
-    <t>R30, R35, R37</t>
+    <t>R34, R39, R41</t>
   </si>
   <si>
     <t>10M</t>
   </si>
   <si>
-    <t>R31, R34</t>
+    <t>R35, R38</t>
   </si>
   <si>
     <t>120, 0.1%</t>
   </si>
   <si>
-    <t>R32</t>
+    <t>R36</t>
   </si>
   <si>
     <t>3.3к</t>
   </si>
   <si>
-    <t>R33</t>
+    <t>R37</t>
   </si>
   <si>
     <t>33к</t>
   </si>
   <si>
-    <t>R42, R43, R185</t>
+    <t>R46, R47, R189</t>
   </si>
   <si>
     <t>4.7к</t>
   </si>
   <si>
-    <t>R44, R61, R62, R63, R69, R70, R71, R77, R78, R79, R85, R86, R87, R93, R94, R95, R100, R103, R106, R109, R112, R113, R114, R119, R120, R121, R212, R213, R216, R217, R245, R247, R250, R252, R272, R274, R277, R279, R284, R285, R288, R289, R317, R319, R322, R324, R344, R346, R349, R351, R_EN2, R_EN4, R_EN6, R_EN8</t>
-  </si>
-  <si>
-    <t>R48, R54, R_EN1, R_EN3, R_EN5, R_EN7, R_FB1, R_FB5</t>
+    <t>R48, R65, R66, R67, R73, R74, R75, R81, R82, R83, R89, R90, R91, R97, R98, R99, R104, R107, R110, R113, R123, R124, R125, R217, R218, R221, R222, R251, R253, R256, R258, R278, R280, R283, R285, R290, R291, R294, R295, R324, R326, R329, R331, R351, R353, R356, R358, R_EN2, R_EN4, R_EN6, R_EN8</t>
+  </si>
+  <si>
+    <t>R52, R58, R_EN1, R_EN3, R_EN5, R_EN7, R_FB1, R_FB5</t>
   </si>
   <si>
     <t>100к</t>
   </si>
   <si>
-    <t>R51</t>
+    <t>R55</t>
   </si>
   <si>
     <t>12к</t>
   </si>
   <si>
-    <t>R52</t>
+    <t>R56</t>
   </si>
   <si>
     <t>110к</t>
   </si>
   <si>
-    <t>R53, R55, R234, R237, R261, R264, R306, R309, R333, R336</t>
+    <t>R57, R59, R206, R240, R243, R267, R270, R313, R316, R340, R343</t>
   </si>
   <si>
     <t>0</t>
   </si>
   <si>
-    <t>R57, R187, R195</t>
+    <t>R61, R191, R199</t>
   </si>
   <si>
     <t>20к</t>
   </si>
   <si>
-    <t>R58</t>
+    <t>R62</t>
   </si>
   <si>
     <t>61к</t>
   </si>
   <si>
-    <t>R59, R67, R75, R83, R91</t>
+    <t>R63, R71, R79, R87, R95</t>
   </si>
   <si>
     <t>10мОм 0.5% 100ppm/°C</t>
   </si>
   <si>
-    <t>R99, R102, R105, R108</t>
-  </si>
-  <si>
-    <t>R101, R104, R107, R110, R127, R131, R133, R135, R138, R141, R144, R147, R150, R153, R156, R159, R162, R165, R168, R171, R174, R177, R180, R197, R198, R232, R240, R243, R246, R254, R259, R267, R270, R273, R281, R304, R312, R315, R318, R326, R331, R339, R342, R345, R353</t>
+    <t>R103, R106, R109, R112</t>
+  </si>
+  <si>
+    <t>R105, R108, R111, R114, R131, R135, R137, R139, R142, R145, R148, R151, R154, R157, R160, R163, R166, R169, R172, R175, R178, R181, R184, R201, R202, R238, R246, R249, R252, R260, R265, R273, R276, R279, R287, R311, R319, R322, R325, R333, R338, R346, R349, R352, R360</t>
   </si>
   <si>
     <t>10</t>
   </si>
   <si>
-    <t>R111, R356</t>
-  </si>
-  <si>
-    <t>10k</t>
-  </si>
-  <si>
-    <t>R129, R132, R134, R139, R145, R151, R157, R163, R169, R175, R181</t>
-  </si>
-  <si>
-    <t>R136, R137, R142, R143, R148, R149, R154, R155, R160, R161, R166, R167, R172, R173, R178, R179, R255, R256, R282, R283, R327, R328, R354, R355</t>
+    <t>R133, R136, R138, R143, R149, R155, R161, R167, R173, R179, R185</t>
+  </si>
+  <si>
+    <t>R140, R141, R146, R147, R152, R153, R158, R159, R164, R165, R170, R171, R176, R177, R182, R183, R261, R262, R288, R289, R334, R335, R361, R362</t>
   </si>
   <si>
     <t>20</t>
   </si>
   <si>
-    <t>R188, R196</t>
+    <t>R192, R200</t>
   </si>
   <si>
     <t>470к</t>
   </si>
   <si>
-    <t>R189, R192, R200, R_FB6, R_FB8</t>
+    <t>R193, R196, R204, R_FB6, R_FB8</t>
   </si>
   <si>
     <t>47к</t>
   </si>
   <si>
-    <t>R191</t>
+    <t>R195</t>
   </si>
   <si>
     <t>5.6к</t>
   </si>
   <si>
-    <t>R193, R201</t>
+    <t>R197, R205</t>
   </si>
   <si>
     <t>1.6к</t>
   </si>
   <si>
-    <t>R202</t>
-  </si>
-  <si>
-    <t>R203</t>
-  </si>
-  <si>
-    <t>R220, R221, R231, R233, R236, R258, R260, R263, R292, R293, R303, R305, R308, R330, R332, R335</t>
+    <t>R225, R226, R237, R239, R242, R264, R266, R269, R298, R299, R310, R312, R315, R337, R339, R342</t>
   </si>
   <si>
     <t>49.9</t>
   </si>
   <si>
-    <t>R228, R300</t>
+    <t>R234, R307</t>
   </si>
   <si>
     <t>1500</t>
   </si>
   <si>
-    <t>R229, R301</t>
+    <t>R235, R308</t>
   </si>
   <si>
     <t>430</t>
@@ -969,7 +997,7 @@
     <t>Y1</t>
   </si>
   <si>
-    <t>XTAL OSC VCXO 100.0000MHZ CMOS</t>
+    <t>XTAL OSC VCXO 50.0000MHZ CMOS</t>
   </si>
   <si>
     <t>CVHD-950-100.000</t>
@@ -988,6 +1016,9 @@
   </si>
   <si>
     <t>SMD_7050_Crystal_Oscillator</t>
+  </si>
+  <si>
+    <t>ы</t>
   </si>
 </sst>
 </file>
@@ -1004,7 +1035,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1017,8 +1048,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1041,16 +1084,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1364,18 +1423,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{269EF48D-6CFC-48D9-A98A-589848DE8865}">
-  <dimension ref="A1:F114"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9EE157B-67BA-4888-948D-8886E7615745}">
+  <dimension ref="A1:G116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="58" customWidth="1"/>
-    <col min="2" max="2" width="33.7109375" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
     <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="35.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1400,22 +1461,22 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="6">
         <v>111</v>
       </c>
     </row>
@@ -1536,7 +1597,7 @@
         <v>25</v>
       </c>
       <c r="F8" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1587,21 +1648,21 @@
         <v>7</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F11" s="1">
-        <v>36</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>7</v>
@@ -1610,7 +1671,7 @@
         <v>8</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>16</v>
@@ -1621,7 +1682,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>7</v>
@@ -1630,7 +1691,7 @@
         <v>8</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>16</v>
@@ -1641,7 +1702,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>7</v>
@@ -1650,10 +1711,10 @@
         <v>8</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F14" s="1">
         <v>1</v>
@@ -1661,7 +1722,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>7</v>
@@ -1670,78 +1731,78 @@
         <v>8</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F15" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F16" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F17" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F18" s="1">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>7</v>
@@ -1750,7 +1811,7 @@
         <v>8</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>10</v>
@@ -1761,7 +1822,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>7</v>
@@ -1770,7 +1831,7 @@
         <v>8</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>10</v>
@@ -1781,7 +1842,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>7</v>
@@ -1790,7 +1851,7 @@
         <v>8</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>16</v>
@@ -1801,7 +1862,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>7</v>
@@ -1810,7 +1871,7 @@
         <v>8</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>16</v>
@@ -1821,7 +1882,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>7</v>
@@ -1830,7 +1891,7 @@
         <v>8</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>16</v>
@@ -1841,7 +1902,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>7</v>
@@ -1850,7 +1911,7 @@
         <v>8</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>16</v>
@@ -1861,7 +1922,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>7</v>
@@ -1870,7 +1931,7 @@
         <v>8</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>16</v>
@@ -1881,7 +1942,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>7</v>
@@ -1890,7 +1951,7 @@
         <v>8</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>16</v>
@@ -1901,7 +1962,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>7</v>
@@ -1910,7 +1971,7 @@
         <v>8</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>16</v>
@@ -1921,75 +1982,77 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>74</v>
+        <v>7</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>75</v>
+        <v>8</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="F28" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="E29" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F29" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D30" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="E30" s="2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="F30" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F31" s="1">
         <v>1</v>
@@ -1997,255 +2060,251 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F32" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D33" s="8"/>
+      <c r="E33" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F33" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="F32" s="1">
+      <c r="B34" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D34" s="6"/>
+      <c r="E34" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F34" s="6">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D33" s="1"/>
-      <c r="E33" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F33" s="1">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D35" s="8"/>
+      <c r="E35" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F35" s="8">
         <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F34" s="1">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F35" s="1">
-        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F36" s="1">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="F37" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="E38" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F38" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>111</v>
-      </c>
       <c r="E39" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F39" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>115</v>
-      </c>
       <c r="E40" s="2" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="F40" s="1">
-        <v>29</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="C41" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>118</v>
-      </c>
       <c r="E41" s="2" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="F41" s="1">
-        <v>40</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>116</v>
-      </c>
       <c r="F42" s="1">
-        <v>12</v>
+        <v>29</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>122</v>
-      </c>
       <c r="E43" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F43" s="1">
-        <v>1</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>125</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="F44" s="1">
         <v>5</v>
@@ -2253,79 +2312,79 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F45" s="1">
-        <v>72</v>
+        <v>12</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F46" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F47" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>116</v>
+        <v>135</v>
       </c>
       <c r="F48" s="1">
         <v>1</v>
@@ -2333,99 +2392,99 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F49" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F50" s="1">
-        <v>3</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>64</v>
+        <v>140</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F51" s="1">
-        <v>54</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F52" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F53" s="1">
         <v>1</v>
@@ -2433,19 +2492,19 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F54" s="1">
         <v>1</v>
@@ -2453,339 +2512,339 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F55" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>148</v>
+        <v>61</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F56" s="1">
-        <v>3</v>
+        <v>51</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F57" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F58" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>64</v>
+        <v>155</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F59" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F60" s="1">
-        <v>45</v>
+        <v>11</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F61" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>122</v>
+        <v>161</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F62" s="1">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="F63" s="1">
-        <v>24</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>162</v>
+        <v>61</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>116</v>
+        <v>135</v>
       </c>
       <c r="F64" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F65" s="1">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>166</v>
+        <v>134</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F66" s="1">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>116</v>
+        <v>135</v>
       </c>
       <c r="F67" s="1">
-        <v>2</v>
+        <v>24</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>146</v>
+        <v>171</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F68" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>125</v>
+        <v>173</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F69" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F70" s="1">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F71" s="1">
         <v>2</v>
@@ -2793,59 +2852,59 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F72" s="1">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F73" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F74" s="1">
         <v>2</v>
@@ -2853,19 +2912,19 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F75" s="1">
         <v>1</v>
@@ -2873,19 +2932,19 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>184</v>
+        <v>116</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>146</v>
+        <v>187</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>185</v>
+        <v>119</v>
       </c>
       <c r="F76" s="1">
         <v>2</v>
@@ -2893,39 +2952,39 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>184</v>
+        <v>116</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>127</v>
+        <v>189</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>185</v>
+        <v>119</v>
       </c>
       <c r="F77" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>64</v>
+        <v>157</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="F78" s="1">
         <v>2</v>
@@ -2933,41 +2992,45 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="D79" s="1"/>
+        <v>117</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>138</v>
+      </c>
       <c r="E79" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="F79" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E80" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B80" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D80" s="1"/>
-      <c r="E80" s="2" t="s">
-        <v>194</v>
-      </c>
       <c r="F80" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>195</v>
       </c>
@@ -2982,10 +3045,10 @@
         <v>198</v>
       </c>
       <c r="F81" s="1">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>199</v>
       </c>
@@ -2997,121 +3060,121 @@
       </c>
       <c r="D82" s="1"/>
       <c r="E82" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F82" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="F82" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="2" t="s">
+      <c r="B83" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="C83" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>205</v>
       </c>
       <c r="D83" s="1"/>
       <c r="E83" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="F83" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="F83" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="2" t="s">
+      <c r="B84" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="C84" s="2" t="s">
         <v>208</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>209</v>
       </c>
       <c r="D84" s="1"/>
       <c r="E84" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F84" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B85" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="C85" s="2" t="s">
         <v>212</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>213</v>
       </c>
       <c r="D85" s="1"/>
       <c r="E85" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F85" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B86" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="C86" s="2" t="s">
         <v>216</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>217</v>
       </c>
       <c r="D86" s="1"/>
       <c r="E86" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F86" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B87" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="C87" s="2" t="s">
         <v>220</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>221</v>
       </c>
       <c r="D87" s="1"/>
       <c r="E87" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F87" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B88" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="C88" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>225</v>
       </c>
       <c r="D88" s="1"/>
       <c r="E88" s="2" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="F88" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>226</v>
       </c>
@@ -3126,10 +3189,10 @@
         <v>229</v>
       </c>
       <c r="F89" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>230</v>
       </c>
@@ -3141,31 +3204,34 @@
       </c>
       <c r="D90" s="1"/>
       <c r="E90" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="F90" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="F90" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
+      <c r="B91" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="C91" s="2" t="s">
         <v>235</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>236</v>
       </c>
       <c r="D91" s="1"/>
       <c r="E91" s="2" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="F91" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="G91" s="9" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>237</v>
       </c>
@@ -3180,10 +3246,10 @@
         <v>240</v>
       </c>
       <c r="F92" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>241</v>
       </c>
@@ -3195,81 +3261,81 @@
       </c>
       <c r="D93" s="1"/>
       <c r="E93" s="2" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="F93" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B94" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="C94" s="2" t="s">
         <v>246</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>247</v>
       </c>
       <c r="D94" s="1"/>
       <c r="E94" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="F94" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="F94" s="1">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="s">
+      <c r="B95" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="C95" s="2" t="s">
         <v>250</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>251</v>
       </c>
       <c r="D95" s="1"/>
       <c r="E95" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="F95" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="F95" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
+      <c r="B96" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="C96" s="2" t="s">
         <v>254</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>255</v>
       </c>
       <c r="D96" s="1"/>
       <c r="E96" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="F96" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="F96" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="2" t="s">
+      <c r="B97" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="C97" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="C97" s="2" t="s">
+      <c r="D97" s="6"/>
+      <c r="E97" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="D97" s="1"/>
-      <c r="E97" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="F97" s="1">
+      <c r="F97" s="6">
         <v>1</v>
       </c>
     </row>
@@ -3303,43 +3369,43 @@
       </c>
       <c r="D99" s="1"/>
       <c r="E99" s="2" t="s">
-        <v>267</v>
+        <v>217</v>
       </c>
       <c r="F99" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B100" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="C100" s="2" t="s">
         <v>269</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>270</v>
       </c>
       <c r="D100" s="1"/>
       <c r="E100" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F100" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B101" s="2" t="s">
         <v>272</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>269</v>
       </c>
       <c r="C101" s="2" t="s">
         <v>273</v>
       </c>
       <c r="D101" s="1"/>
       <c r="E101" s="2" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="F101" s="1">
         <v>4</v>
@@ -3347,38 +3413,38 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D102" s="1"/>
       <c r="E102" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F102" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>280</v>
       </c>
       <c r="D103" s="1"/>
       <c r="E103" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F103" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
@@ -3393,45 +3459,45 @@
       </c>
       <c r="D104" s="1"/>
       <c r="E104" s="2" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F104" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="B105" s="2" t="s">
+      <c r="A105" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="C105" s="2" t="s">
+      <c r="B105" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="D105" s="1"/>
-      <c r="E105" s="2" t="s">
+      <c r="C105" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="F105" s="1">
-        <v>10</v>
+      <c r="D105" s="6"/>
+      <c r="E105" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="F105" s="6">
+        <v>7</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="2" t="s">
+      <c r="A106" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="B106" s="2" t="s">
+      <c r="B106" s="7" t="s">
         <v>289</v>
       </c>
-      <c r="C106" s="2" t="s">
+      <c r="C106" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="D106" s="1"/>
-      <c r="E106" s="2" t="s">
+      <c r="D106" s="8"/>
+      <c r="E106" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="F106" s="1">
+      <c r="F106" s="8">
         <v>1</v>
       </c>
     </row>
@@ -3450,7 +3516,7 @@
         <v>294</v>
       </c>
       <c r="F107" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
@@ -3465,25 +3531,25 @@
       </c>
       <c r="D108" s="1"/>
       <c r="E108" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F108" s="1">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B109" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="C109" s="2" t="s">
         <v>300</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>301</v>
       </c>
       <c r="D109" s="1"/>
       <c r="E109" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F109" s="1">
         <v>1</v>
@@ -3491,91 +3557,127 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B110" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="B110" s="2" t="s">
+      <c r="C110" s="2" t="s">
         <v>304</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>305</v>
       </c>
       <c r="D110" s="1"/>
       <c r="E110" s="2" t="s">
         <v>305</v>
       </c>
       <c r="F110" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="C111" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="D111" s="6"/>
+      <c r="E111" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="F111" s="6">
         <v>1</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="D111" s="1"/>
-      <c r="E111" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="F111" s="1">
-        <v>5</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="D112" s="1"/>
       <c r="E112" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F112" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C113" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D113" s="1"/>
       <c r="E113" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F113" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B114" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="C114" s="2" t="s">
         <v>317</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>318</v>
       </c>
       <c r="D114" s="1"/>
       <c r="E114" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="F114" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="F114" s="1">
+      <c r="B115" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D115" s="1"/>
+      <c r="E115" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="F115" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="D116" s="1"/>
+      <c r="E116" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="F116" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
0.53 add flex-borders layer (M10)
</commit_message>
<xml_diff>
--- a/Project Outputs for llrf_afe/BOM/llrf_afe.xlsx
+++ b/Project Outputs for llrf_afe/BOM/llrf_afe.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YandexDisk\Work\Altium\COSY\llrf_afe\Project Outputs for llrf_afe\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3B685A-6707-4297-9740-A2090BDED083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E2AD221-11B7-41FB-B2F5-3DB0FBEAB22B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13755" yWindow="2835" windowWidth="28110" windowHeight="15885" xr2:uid="{C09BF35C-D0E0-45A9-B6AD-F4DB426FEBD2}"/>
+    <workbookView xWindow="45705" yWindow="3405" windowWidth="28110" windowHeight="15885" xr2:uid="{74BD8172-CEA3-42A8-B072-D67FA12BADE2}"/>
   </bookViews>
   <sheets>
     <sheet name="llrf_afe" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">llrf_afe!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="328">
   <si>
     <t>Designator</t>
   </si>
@@ -70,10 +70,10 @@
     <t>SMD_C0402</t>
   </si>
   <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>0.33мкФ</t>
+    <t>C2, C93, C297, C298</t>
+  </si>
+  <si>
+    <t>SMD_C0603</t>
   </si>
   <si>
     <t>C3, C4, C5, C6, C29, C30, C31, C32, C209, C215, C216, C226, C232, C233, C266, C272, C273, C283, C289, C290</t>
@@ -85,9 +85,6 @@
     <t>1мкФ 6.3В X7T</t>
   </si>
   <si>
-    <t>SMD_C0603</t>
-  </si>
-  <si>
     <t>C7, C201, C258</t>
   </si>
   <si>
@@ -151,9 +148,6 @@
     <t>10мкФ 16В</t>
   </si>
   <si>
-    <t>C93</t>
-  </si>
-  <si>
     <t>C98, C99, C100</t>
   </si>
   <si>
@@ -835,7 +829,10 @@
     <t>Programmable NOR flash memory</t>
   </si>
   <si>
-    <t>EPCQ32SI8N</t>
+    <t>S25FL128SAGNFV000</t>
+  </si>
+  <si>
+    <t>WSON-8_6x8</t>
   </si>
   <si>
     <t>U34, U41</t>
@@ -874,7 +871,7 @@
     <t>SOD-323</t>
   </si>
   <si>
-    <t>VD4, VD5, VD16, VD17</t>
+    <t>VD4, VD5</t>
   </si>
   <si>
     <t>PESDxL1BA</t>
@@ -892,6 +889,12 @@
     <t>SOT-23</t>
   </si>
   <si>
+    <t>VD16, VD17</t>
+  </si>
+  <si>
+    <t>PESD5V0L1BA</t>
+  </si>
+  <si>
     <t>X1, X2, X3, X4, X8, X9, X11</t>
   </si>
   <si>
@@ -1009,16 +1012,13 @@
     <t>Y2</t>
   </si>
   <si>
-    <t>Crystall oscillator, CMOS, 3.3V, SMD7050</t>
+    <t>Crystall oscillator, CMOS, 3.3V, SMD7050, 100 МГц</t>
   </si>
   <si>
     <t>XG-1000CA</t>
   </si>
   <si>
     <t>SMD_7050_Crystal_Oscillator</t>
-  </si>
-  <si>
-    <t>ы</t>
   </si>
 </sst>
 </file>
@@ -1035,7 +1035,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1048,20 +1048,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1084,32 +1072,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1423,20 +1395,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9EE157B-67BA-4888-948D-8886E7615745}">
-  <dimension ref="A1:G116"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3C713D6-1AD2-4EF5-887D-ADEA3FA600C2}">
+  <dimension ref="A1:F116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="58" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
     <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="35.42578125" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1461,22 +1431,22 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="1">
         <v>111</v>
       </c>
     </row>
@@ -1491,13 +1461,13 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="F3" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1514,7 +1484,7 @@
         <v>15</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F4" s="1">
         <v>20</v>
@@ -1522,7 +1492,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>7</v>
@@ -1531,7 +1501,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>10</v>
@@ -1542,7 +1512,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>7</v>
@@ -1551,7 +1521,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>10</v>
@@ -1562,19 +1532,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="F7" s="1">
         <v>7</v>
@@ -1582,19 +1552,19 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F8" s="1">
         <v>27</v>
@@ -1602,19 +1572,19 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="F9" s="1">
         <v>2</v>
@@ -1622,7 +1592,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>7</v>
@@ -1631,10 +1601,10 @@
         <v>8</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="F10" s="1">
         <v>8</v>
@@ -1642,7 +1612,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>7</v>
@@ -1651,10 +1621,10 @@
         <v>8</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F11" s="1">
         <v>12</v>
@@ -1662,7 +1632,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>7</v>
@@ -1671,13 +1641,13 @@
         <v>8</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F12" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1694,15 +1664,15 @@
         <v>40</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="F13" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>7</v>
@@ -1711,13 +1681,13 @@
         <v>8</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="F14" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1725,19 +1695,19 @@
         <v>44</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="F15" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1745,19 +1715,19 @@
         <v>46</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>47</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="F16" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1768,16 +1738,16 @@
         <v>7</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F17" s="1">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1788,16 +1758,16 @@
         <v>7</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="E18" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F18" s="1">
-        <v>25</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1817,7 +1787,7 @@
         <v>10</v>
       </c>
       <c r="F19" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1834,10 +1804,10 @@
         <v>55</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F20" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1854,7 +1824,7 @@
         <v>57</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F21" s="1">
         <v>2</v>
@@ -1874,10 +1844,10 @@
         <v>59</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F22" s="1">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1894,10 +1864,10 @@
         <v>61</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F23" s="1">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1914,10 +1884,10 @@
         <v>63</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F24" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1934,7 +1904,7 @@
         <v>65</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F25" s="1">
         <v>8</v>
@@ -1954,7 +1924,7 @@
         <v>67</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F26" s="1">
         <v>8</v>
@@ -1974,10 +1944,10 @@
         <v>69</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F27" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1985,39 +1955,39 @@
         <v>70</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="F28" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C29" s="2" t="s">
+      <c r="D29" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="F29" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -2025,34 +1995,32 @@
         <v>77</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>78</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="D30" s="1"/>
       <c r="E30" s="2" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F30" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F31" s="1">
         <v>1</v>
@@ -2060,114 +2028,116 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F32" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="C33" s="7" t="s">
+      <c r="A33" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D33" s="8"/>
-      <c r="E33" s="7" t="s">
+      <c r="B33" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F33" s="8">
-        <v>1</v>
+      <c r="C33" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F33" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C34" s="5" t="s">
+      <c r="A34" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D34" s="6"/>
-      <c r="E34" s="5" t="s">
+      <c r="B34" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F34" s="6">
-        <v>4</v>
+      <c r="C34" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D34" s="1"/>
+      <c r="E34" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F34" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="B35" s="7" t="s">
+      <c r="A35" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="B35" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D35" s="8"/>
-      <c r="E35" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="F35" s="8">
-        <v>2</v>
+      <c r="C35" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F35" s="1">
+        <v>21</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F36" s="1">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="F37" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -2175,16 +2145,16 @@
         <v>107</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>108</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F38" s="1">
         <v>8</v>
@@ -2195,19 +2165,19 @@
         <v>109</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>110</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F39" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -2215,16 +2185,16 @@
         <v>111</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>112</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F40" s="1">
         <v>4</v>
@@ -2235,39 +2205,39 @@
         <v>113</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="F41" s="1">
-        <v>4</v>
+        <v>29</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C42" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="F42" s="1">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -2275,39 +2245,39 @@
         <v>120</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="F43" s="1">
-        <v>38</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="F44" s="1">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -2315,19 +2285,19 @@
         <v>127</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>128</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F45" s="1">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -2335,19 +2305,19 @@
         <v>129</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>130</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F46" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2355,59 +2325,59 @@
         <v>131</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>132</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="F47" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C48" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D48" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>135</v>
-      </c>
       <c r="F48" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C49" s="2" t="s">
+      <c r="E49" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D49" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="F49" s="1">
-        <v>6</v>
+        <v>72</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -2415,19 +2385,19 @@
         <v>137</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>138</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F50" s="1">
-        <v>72</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -2435,19 +2405,19 @@
         <v>139</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>140</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F51" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -2455,19 +2425,19 @@
         <v>141</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>142</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F52" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -2475,16 +2445,16 @@
         <v>143</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>144</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F53" s="1">
         <v>1</v>
@@ -2495,19 +2465,19 @@
         <v>145</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>146</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F54" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -2515,39 +2485,39 @@
         <v>147</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C55" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E55" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D55" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="F55" s="1">
-        <v>3</v>
+        <v>51</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B56" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C56" s="2" t="s">
+      <c r="E56" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D56" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="F56" s="1">
-        <v>51</v>
+        <v>8</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -2555,19 +2525,19 @@
         <v>150</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>151</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F57" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -2575,16 +2545,16 @@
         <v>152</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>153</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F58" s="1">
         <v>1</v>
@@ -2595,19 +2565,19 @@
         <v>154</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>155</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F59" s="1">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -2615,19 +2585,19 @@
         <v>156</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>157</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F60" s="1">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -2635,19 +2605,19 @@
         <v>158</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>159</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F61" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -2655,19 +2625,19 @@
         <v>160</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>161</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="F62" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -2675,39 +2645,39 @@
         <v>162</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>163</v>
+        <v>59</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F63" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D64" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B64" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C64" s="2" t="s">
+      <c r="E64" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D64" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>135</v>
-      </c>
       <c r="F64" s="1">
-        <v>4</v>
+        <v>45</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -2715,39 +2685,39 @@
         <v>165</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C65" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E65" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D65" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="F65" s="1">
-        <v>45</v>
+        <v>11</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D66" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B66" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="E66" s="2" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="F66" s="1">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -2755,19 +2725,19 @@
         <v>168</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>169</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="F67" s="1">
-        <v>24</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -2775,19 +2745,19 @@
         <v>170</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>171</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F68" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -2795,19 +2765,19 @@
         <v>172</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>173</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F69" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -2815,19 +2785,19 @@
         <v>174</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>175</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F70" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -2835,19 +2805,19 @@
         <v>176</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>177</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F71" s="1">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -2855,19 +2825,19 @@
         <v>178</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>179</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F72" s="1">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -2875,16 +2845,16 @@
         <v>180</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>181</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F73" s="1">
         <v>2</v>
@@ -2895,19 +2865,19 @@
         <v>182</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>183</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F74" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -2915,19 +2885,19 @@
         <v>184</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>185</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F75" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -2935,19 +2905,19 @@
         <v>186</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>187</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F76" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -2955,36 +2925,36 @@
         <v>188</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>116</v>
+        <v>189</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>189</v>
+        <v>155</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>119</v>
+        <v>190</v>
       </c>
       <c r="F77" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E78" s="2" t="s">
         <v>190</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>192</v>
       </c>
       <c r="F78" s="1">
         <v>2</v>
@@ -2992,19 +2962,19 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>138</v>
+        <v>59</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F79" s="1">
         <v>2</v>
@@ -3012,508 +2982,503 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B80" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="B80" s="2" t="s">
-        <v>191</v>
-      </c>
       <c r="C80" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>61</v>
-      </c>
+        <v>195</v>
+      </c>
+      <c r="D80" s="1"/>
       <c r="E80" s="2" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="F80" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D81" s="1"/>
       <c r="E81" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F81" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D82" s="1"/>
       <c r="E82" s="2" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="F82" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D83" s="1"/>
       <c r="E83" s="2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="F83" s="1">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="D84" s="1"/>
       <c r="E84" s="2" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="F84" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="D85" s="1"/>
       <c r="E85" s="2" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="F85" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D86" s="1"/>
       <c r="E86" s="2" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="F86" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D87" s="1"/>
       <c r="E87" s="2" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="F87" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="D88" s="1"/>
       <c r="E88" s="2" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="F88" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="D89" s="1"/>
       <c r="E89" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F89" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D90" s="1"/>
       <c r="E90" s="2" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="F90" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D91" s="1"/>
       <c r="E91" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="F91" s="1">
-        <v>5</v>
-      </c>
-      <c r="G91" s="9" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="D92" s="1"/>
       <c r="E92" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F92" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D93" s="1"/>
       <c r="E93" s="2" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="F93" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="D94" s="1"/>
       <c r="E94" s="2" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="F94" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="D95" s="1"/>
       <c r="E95" s="2" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="F95" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="D96" s="1"/>
       <c r="E96" s="2" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="F96" s="1">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="B97" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="C97" s="5" t="s">
+      <c r="A97" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="D97" s="6"/>
-      <c r="E97" s="5" t="s">
+      <c r="B97" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="F97" s="6">
-        <v>1</v>
+      <c r="C97" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="D97" s="1"/>
+      <c r="E97" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="F97" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="D98" s="1"/>
       <c r="E98" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="F98" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="D99" s="1"/>
       <c r="E99" s="2" t="s">
-        <v>217</v>
+        <v>269</v>
       </c>
       <c r="F99" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="D100" s="1"/>
       <c r="E100" s="2" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="F100" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="D101" s="1"/>
       <c r="E101" s="2" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="F101" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B102" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="B102" s="2" t="s">
-        <v>276</v>
-      </c>
       <c r="C102" s="2" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D102" s="1"/>
       <c r="E102" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F102" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="D103" s="1"/>
       <c r="E103" s="2" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="F103" s="1">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="D104" s="1"/>
       <c r="E104" s="2" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="F104" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="B105" s="5" t="s">
+      <c r="A105" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="C105" s="5" t="s">
+      <c r="B105" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="D105" s="6"/>
-      <c r="E105" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="F105" s="6">
+      <c r="C105" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="D105" s="1"/>
+      <c r="E105" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="F105" s="1">
         <v>7</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="B106" s="7" t="s">
+      <c r="A106" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="C106" s="7" t="s">
+      <c r="B106" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="D106" s="8"/>
-      <c r="E106" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="F106" s="8">
+      <c r="C106" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D106" s="1"/>
+      <c r="E106" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="F106" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D107" s="1"/>
       <c r="E107" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F107" s="1">
         <v>10</v>
@@ -3521,17 +3486,17 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D108" s="1"/>
       <c r="E108" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="F108" s="1">
         <v>1</v>
@@ -3539,17 +3504,17 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D109" s="1"/>
       <c r="E109" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="F109" s="1">
         <v>1</v>
@@ -3557,53 +3522,53 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D110" s="1"/>
       <c r="E110" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="F110" s="1">
         <v>13</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" s="5" t="s">
-        <v>306</v>
-      </c>
-      <c r="B111" s="5" t="s">
+      <c r="A111" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="C111" s="5" t="s">
+      <c r="B111" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="D111" s="6"/>
-      <c r="E111" s="5" t="s">
+      <c r="C111" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="F111" s="6">
+      <c r="D111" s="1"/>
+      <c r="E111" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="F111" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D112" s="1"/>
       <c r="E112" s="2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="F112" s="1">
         <v>1</v>
@@ -3611,17 +3576,17 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D113" s="1"/>
       <c r="E113" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="F113" s="1">
         <v>5</v>
@@ -3629,17 +3594,17 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D114" s="1"/>
       <c r="E114" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="F114" s="1">
         <v>8</v>
@@ -3647,17 +3612,17 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D115" s="1"/>
       <c r="E115" s="2" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="F115" s="1">
         <v>1</v>
@@ -3665,17 +3630,17 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D116" s="1"/>
       <c r="E116" s="2" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="F116" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
0.53.1 change project version to 0.53
</commit_message>
<xml_diff>
--- a/Project Outputs for llrf_afe/BOM/llrf_afe.xlsx
+++ b/Project Outputs for llrf_afe/BOM/llrf_afe.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YandexDisk\Work\Altium\COSY\llrf_afe\Project Outputs for llrf_afe\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E2AD221-11B7-41FB-B2F5-3DB0FBEAB22B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9C36617-0979-422B-8243-0893AC7E7CE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45705" yWindow="3405" windowWidth="28110" windowHeight="15885" xr2:uid="{74BD8172-CEA3-42A8-B072-D67FA12BADE2}"/>
+    <workbookView xWindow="6720" yWindow="3780" windowWidth="28110" windowHeight="15885" xr2:uid="{DF7355B2-25C5-4BF9-8E9C-85DD0256A1EC}"/>
   </bookViews>
   <sheets>
     <sheet name="llrf_afe" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">llrf_afe!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1395,7 +1395,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3C713D6-1AD2-4EF5-887D-ADEA3FA600C2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E90A73E3-D209-4859-A4A1-8FA39F88837D}">
   <dimension ref="A1:F116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
0.7.0 remove the flex-pcb part and the reserve FMC connector
</commit_message>
<xml_diff>
--- a/Project Outputs for llrf_afe/BOM/llrf_afe.xlsx
+++ b/Project Outputs for llrf_afe/BOM/llrf_afe.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YandexDisk\Work\Altium\COSY\llrf_afe\Project Outputs for llrf_afe\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9C36617-0979-422B-8243-0893AC7E7CE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{26CC9466-6E28-48C1-ABBF-0388BD2E04DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6720" yWindow="3780" windowWidth="28110" windowHeight="15885" xr2:uid="{DF7355B2-25C5-4BF9-8E9C-85DD0256A1EC}"/>
+    <workbookView xWindow="65145" yWindow="15195" windowWidth="11655" windowHeight="7980" xr2:uid="{E630B9FC-66F4-4D88-ABF0-1CC1E4D340C0}"/>
   </bookViews>
   <sheets>
     <sheet name="llrf_afe" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">llrf_afe!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,8 +26,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="341">
   <si>
     <t>Designator</t>
   </si>
@@ -55,7 +58,7 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>C1, C8, C9, C10, C11, C16, C17, C18, C19, C20, C22, C24, C26, C27, C28, C52, C54, C55, C56, C57, C58, C60, C61, C62, C63, C82, C83, C85, C87, C89, C91, C92, C94, C95, C96, C97, C102, C104, C105, C108, C109, C111, C114, C128, C129, C130, C131, C132, C145, C146, C148, C150, C152, C154, C156, C158, C160, C162, C164, C167, C169, C177, C178, C179, C180, C181, C183, C184, C187, C188, C191, C193, C194, C195, C196, C197, C198, C199, C200, C208, C214, C217, C218, C225, C231, C234, C235, C236, C237, C238, C240, C241, C244, C245, C248, C250, C251, C252, C253, C254, C255, C256, C257, C265, C271, C274, C275, C282, C288, C291, C292</t>
+    <t>C1, C10, C11, C12, C13, C18, C19, C20, C21, C22, C24, C26, C28, C29, C30, C54, C56, C57, C58, C59, C60, C62, C63, C64, C65, C84, C85, C87, C89, C91, C93, C94, C96, C97, C98, C99, C104, C106, C107, C110, C111, C113, C116, C130, C131, C132, C133, C134, C159, C160, C162, C164, C166, C168, C170, C172, C174, C176, C178, C181, C183, C191, C192, C193, C194, C195, C197, C198, C201, C202, C205, C207, C208, C209, C210, C211, C212, C213, C214, C222, C228, C231, C232, C239, C245, C248, C249, C250, C251, C252, C254, C255, C258, C259, C262, C264, C265, C266, C267, C268, C269, C270, C271, C279, C285, C288, C289, C296, C302, C305, C306</t>
   </si>
   <si>
     <t>SMD-конденсатор</t>
@@ -70,13 +73,13 @@
     <t>SMD_C0402</t>
   </si>
   <si>
-    <t>C2, C93, C297, C298</t>
+    <t>C2, C3, C4, C95</t>
   </si>
   <si>
     <t>SMD_C0603</t>
   </si>
   <si>
-    <t>C3, C4, C5, C6, C29, C30, C31, C32, C209, C215, C216, C226, C232, C233, C266, C272, C273, C283, C289, C290</t>
+    <t>C5, C6, C7, C8, C31, C32, C33, C34, C223, C229, C230, C240, C246, C247, C280, C286, C287, C297, C303, C304</t>
   </si>
   <si>
     <t>GRM033D70J105ME01</t>
@@ -85,19 +88,19 @@
     <t>1мкФ 6.3В X7T</t>
   </si>
   <si>
-    <t>C7, C201, C258</t>
+    <t>C9, C215, C272</t>
   </si>
   <si>
     <t>1нФ</t>
   </si>
   <si>
-    <t>C12, C13</t>
+    <t>C14, C15</t>
   </si>
   <si>
     <t>0.47мкФ</t>
   </si>
   <si>
-    <t>C14, C15, C21, C23, C25, C50, C51</t>
+    <t>C16, C17, C23, C25, C27, C52, C53</t>
   </si>
   <si>
     <t>3 Terminals Low ESL Chip Multilayer Ceramic Capacitors (EMIFIL) for General Purpose</t>
@@ -112,13 +115,13 @@
     <t>3pol_SMD0402</t>
   </si>
   <si>
-    <t>C33, C34, C35, C36, C37, C38, C39, C40, C41, C42, C43, C44, C45, C46, C47, C48, C49, C64, C65, C66, C67, C68, C69, C70, C71, C72, C73</t>
+    <t>C35, C36, C37, C38, C39, C40, C41, C42, C43, C44, C45, C46, C47, C48, C49, C50, C51, C66, C67, C68, C69, C70, C71, C72, C73, C74, C307</t>
   </si>
   <si>
     <t>NFM15PC104D0J3</t>
   </si>
   <si>
-    <t>C53, C59</t>
+    <t>C55, C61</t>
   </si>
   <si>
     <t>Поляризованный SMD-конденсатор</t>
@@ -133,7 +136,7 @@
     <t>SMD_size_B</t>
   </si>
   <si>
-    <t>C74, C75, C76, C77, C78, C79, C80, C81</t>
+    <t>C76, C77, C78, C79, C80, C81, C82, C83</t>
   </si>
   <si>
     <t>1нФ 2кВ</t>
@@ -142,19 +145,19 @@
     <t>SMD_C1206</t>
   </si>
   <si>
-    <t>C84, C86, C88, C90, C103, C106, C107, C110, C112, C113, C115, C116</t>
+    <t>C86, C88, C90, C92, C105, C108, C109, C112, C114, C115, C117, C118</t>
   </si>
   <si>
     <t>10мкФ 16В</t>
   </si>
   <si>
-    <t>C98, C99, C100</t>
+    <t>C100, C101, C102</t>
   </si>
   <si>
     <t>33нФ</t>
   </si>
   <si>
-    <t>C101</t>
+    <t>C103</t>
   </si>
   <si>
     <t>47мкФ</t>
@@ -163,91 +166,115 @@
     <t>SMD_C0805</t>
   </si>
   <si>
-    <t>C117, C119, C122, C123, C124, C125, C126, C127</t>
+    <t>C119, C121, C124, C125, C126, C127, C128, C129</t>
   </si>
   <si>
     <t>2.2мкФ</t>
   </si>
   <si>
-    <t>C118, C120, C121, C170, C171, C174</t>
+    <t>C120, C122, C123, C184, C185, C188</t>
   </si>
   <si>
     <t>10мкФх50В</t>
   </si>
   <si>
-    <t>C133, C134, C136, C137, C139, C140, C142, C143</t>
-  </si>
-  <si>
-    <t>0.22мкФ 25В X7R</t>
-  </si>
-  <si>
-    <t>C135, C138, C141, C144, C147, C149, C151, C153, C155, C157, C159, C161, C163, C182, C185, C186, C189, C190, C192, C239, C242, C243, C246, C247, C249</t>
+    <t>C135, C141, C147, C153</t>
+  </si>
+  <si>
+    <t>0.22мкФ 25В</t>
+  </si>
+  <si>
+    <t>C136, C137, C138, C142, C143, C144, C148, C149, C150, C154, C155, C156</t>
+  </si>
+  <si>
+    <t>22мкФ</t>
+  </si>
+  <si>
+    <t>C139, C145, C151, C157</t>
+  </si>
+  <si>
+    <t>10мкФ</t>
+  </si>
+  <si>
+    <t>C140, C146, C152, C158</t>
+  </si>
+  <si>
+    <t>330нФ</t>
+  </si>
+  <si>
+    <t>C161, C163, C165, C167, C169, C171, C173, C175, C177, C196, C199, C200, C203, C204, C206, C253, C256, C257, C260, C261, C263</t>
   </si>
   <si>
     <t>GRM188C81C106MA73</t>
   </si>
   <si>
-    <t>C165, C166</t>
+    <t>C179, C180</t>
   </si>
   <si>
     <t>47пФ</t>
   </si>
   <si>
-    <t>C168</t>
+    <t>C182</t>
   </si>
   <si>
     <t>10нФ</t>
   </si>
   <si>
-    <t>C172, C175</t>
+    <t>C186, C189</t>
   </si>
   <si>
     <t>2.4нФ</t>
   </si>
   <si>
-    <t>C173, C176</t>
+    <t>C187, C190</t>
   </si>
   <si>
     <t>16нФ</t>
   </si>
   <si>
-    <t>C202, C211, C213, C219, C228, C230, C259, C268, C270, C276, C285, C287</t>
+    <t>C216, C225, C227, C233, C242, C244, C273, C282, C284, C290, C299, C301</t>
   </si>
   <si>
     <t>NU</t>
   </si>
   <si>
-    <t>C203, C220, C260, C277</t>
+    <t>C217, C234, C274, C291</t>
   </si>
   <si>
     <t>13пФ</t>
   </si>
   <si>
-    <t>C204, C205, C221, C222, C261, C262, C278, C279</t>
+    <t>C218, C219, C235, C236, C275, C276, C292, C293</t>
   </si>
   <si>
     <t>32пФ</t>
   </si>
   <si>
-    <t>C206, C207, C223, C224, C263, C264, C280, C281</t>
+    <t>C220, C221, C237, C238, C277, C278, C294, C295</t>
   </si>
   <si>
     <t>91пФ</t>
   </si>
   <si>
-    <t>C210, C212, C227, C229, C267, C269, C284, C286</t>
+    <t>C224, C226, C241, C243, C281, C283, C298, C300</t>
   </si>
   <si>
     <t>62пФ</t>
   </si>
   <si>
-    <t>C293, C294, C295, C296</t>
-  </si>
-  <si>
-    <t>10мкФ 16В X7R</t>
-  </si>
-  <si>
-    <t>D1, D2, D3, D4, D5</t>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>Circuit Board Indicator</t>
+  </si>
+  <si>
+    <t>WP130WCP/2EGW</t>
+  </si>
+  <si>
+    <t>WP130WCP</t>
+  </si>
+  <si>
+    <t>D2, D3, D4, D5, D6</t>
   </si>
   <si>
     <t>Светодиод</t>
@@ -262,13 +289,13 @@
     <t>LED-0805</t>
   </si>
   <si>
-    <t>D6, D7</t>
+    <t>D7, D8</t>
   </si>
   <si>
     <t>red</t>
   </si>
   <si>
-    <t>D8</t>
+    <t>D9</t>
   </si>
   <si>
     <t>4 CHANNEL LOW CAPACITANCE TVS DIODE ARRAY</t>
@@ -280,18 +307,6 @@
     <t>SOT-363</t>
   </si>
   <si>
-    <t>D9</t>
-  </si>
-  <si>
-    <t>Circuit Board Indicator</t>
-  </si>
-  <si>
-    <t>WP130WCP/2EGW</t>
-  </si>
-  <si>
-    <t>WP130WCP</t>
-  </si>
-  <si>
     <t>G1</t>
   </si>
   <si>
@@ -304,19 +319,7 @@
     <t>TDN_5_WISM</t>
   </si>
   <si>
-    <t>G2, G3, G4, G5</t>
-  </si>
-  <si>
-    <t>17-V Input 3-A Step-Down Converter MicroSiP™ Module with Integrated Inductor</t>
-  </si>
-  <si>
-    <t>TPS82130</t>
-  </si>
-  <si>
-    <t>uSiL-8</t>
-  </si>
-  <si>
-    <t>J1, J2</t>
+    <t>J1</t>
   </si>
   <si>
     <t>FMC HPC socket Array Assembly, Surface Mount, 0.050" Pitch, 400 Pins</t>
@@ -325,7 +328,7 @@
     <t>ASP-134488-01</t>
   </si>
   <si>
-    <t>L1, L2, L3, L4, L5, L6, L7, L8, L10, L11, L12, L13, L14, L15, L16, L17, L18, L31, L32, L33, L34</t>
+    <t>L1, L2, L3, L4, L5, L6, L7, L8, L10, L11, L12, L17, L18, L19, L20, L21, L22, L35, L36, L37, L38</t>
   </si>
   <si>
     <t>SMD-индуктивность</t>
@@ -352,31 +355,40 @@
     <t>SDR0805</t>
   </si>
   <si>
-    <t>L19, L20, L25, L26, L35, L36, L41, L42</t>
+    <t>L13, L14, L15, L16</t>
+  </si>
+  <si>
+    <t>2.2мкГн</t>
+  </si>
+  <si>
+    <t>SMD_1210</t>
+  </si>
+  <si>
+    <t>L23, L24, L29, L30, L39, L40, L45, L46</t>
   </si>
   <si>
     <t>50нГн</t>
   </si>
   <si>
-    <t>L21, L22, L27, L28, L37, L38, L43, L44</t>
+    <t>L25, L26, L31, L32, L41, L42, L47, L48</t>
   </si>
   <si>
     <t>110нГн</t>
   </si>
   <si>
-    <t>L23, L29, L39, L45</t>
+    <t>L27, L33, L43, L49</t>
   </si>
   <si>
     <t>200нГн</t>
   </si>
   <si>
-    <t>L24, L30, L40, L46</t>
+    <t>L28, L34, L44, L50</t>
   </si>
   <si>
     <t>130нГн</t>
   </si>
   <si>
-    <t>R1, R4, R5, R6, R33, R40, R45, R198, R211, R241, R244, R247, R248, R250, R268, R271, R274, R275, R277, R314, R317, R320, R321, R323, R341, R344, R347, R348, R350</t>
+    <t>R1, R4, R5, R6, R37, R44, R49, R191, R192, R204, R217, R247, R250, R253, R254, R256, R274, R277, R280, R281, R283, R320, R323, R326, R327, R329, R347, R350, R353, R354, R356</t>
   </si>
   <si>
     <t>SMD-резистор</t>
@@ -391,13 +403,13 @@
     <t>SMD_0603</t>
   </si>
   <si>
-    <t>R2, R3, R8, R10, R12, R14, R15, R16, R17, R18, R19, R21, R22, R23, R25, R28, R44, R68, R69, R70, R76, R77, R78, R84, R85, R86, R92, R93, R94, R100, R101, R102, R120, R127, R236, R263, R309, R336</t>
+    <t>R2, R3, R9, R10, R12, R14, R15, R16, R17, R18, R20, R21, R23, R24, R25, R31, R48, R72, R73, R74, R80, R81, R82, R88, R89, R90, R96, R97, R98, R104, R105, R106, R124, R131, R242, R269, R315, R342</t>
   </si>
   <si>
     <t>100</t>
   </si>
   <si>
-    <t>R7, R9, R11, R13, R208</t>
+    <t>R7, R8, R11, R13, R22, R214</t>
   </si>
   <si>
     <t>4 Chip Resistor Array</t>
@@ -412,193 +424,217 @@
     <t>TC124</t>
   </si>
   <si>
-    <t>R20, R130, R132, R134, R144, R150, R156, R162, R168, R174, R180, R186</t>
+    <t>R19, R134, R136, R138, R148, R154, R160, R166, R172, R178, R184, R190</t>
   </si>
   <si>
     <t>200</t>
   </si>
   <si>
-    <t>R24</t>
+    <t>R26</t>
+  </si>
+  <si>
+    <t>1M</t>
+  </si>
+  <si>
+    <t>SMD_1206</t>
+  </si>
+  <si>
+    <t>R27, R28, R29, R30</t>
+  </si>
+  <si>
+    <t>240</t>
+  </si>
+  <si>
+    <t>R32, R46, R47, R193, R194, R212, R213</t>
+  </si>
+  <si>
+    <t>R33</t>
   </si>
   <si>
     <t>10k</t>
   </si>
   <si>
-    <t>R26, R115, R116, R117</t>
-  </si>
-  <si>
-    <t>240</t>
-  </si>
-  <si>
-    <t>R27</t>
-  </si>
-  <si>
-    <t>1M</t>
-  </si>
-  <si>
-    <t>SMD_1206</t>
-  </si>
-  <si>
-    <t>R29, R42, R43, R187, R188, R207</t>
-  </si>
-  <si>
-    <t>R30, R31, R32, R49, R50, R51, R53, R54, R60, R64, R72, R80, R88, R96, R119, R121, R122, R126, R128, R129, R190, R194, R203, R209, R210, R212, R213, R214, R215, R216, R219, R220, R223, R224, R227, R228, R229, R230, R231, R232, R233, R245, R254, R255, R257, R259, R272, R281, R282, R284, R286, R292, R293, R296, R297, R300, R301, R302, R303, R304, R305, R306, R318, R327, R328, R330, R332, R345, R354, R355, R357, R359</t>
+    <t>R34, R35, R36, R53, R54, R55, R57, R58, R64, R68, R76, R84, R92, R100, R123, R125, R126, R130, R132, R133, R196, R200, R209, R215, R216, R218, R219, R220, R221, R222, R225, R226, R229, R230, R233, R234, R235, R236, R237, R238, R239, R251, R260, R261, R263, R265, R278, R287, R288, R290, R292, R298, R299, R302, R303, R306, R307, R308, R309, R310, R311, R312, R324, R333, R334, R336, R338, R351, R360, R361, R363, R365</t>
   </si>
   <si>
     <t>10к</t>
   </si>
   <si>
-    <t>R34, R39, R41</t>
+    <t>R38, R43, R45</t>
   </si>
   <si>
     <t>10M</t>
   </si>
   <si>
-    <t>R35, R38</t>
+    <t>R39, R42</t>
   </si>
   <si>
     <t>120, 0.1%</t>
   </si>
   <si>
-    <t>R36</t>
+    <t>R40</t>
   </si>
   <si>
     <t>3.3к</t>
   </si>
   <si>
-    <t>R37</t>
+    <t>R41</t>
   </si>
   <si>
     <t>33к</t>
   </si>
   <si>
-    <t>R46, R47, R189</t>
+    <t>R50, R51, R195</t>
   </si>
   <si>
     <t>4.7к</t>
   </si>
   <si>
-    <t>R48, R65, R66, R67, R73, R74, R75, R81, R82, R83, R89, R90, R91, R97, R98, R99, R104, R107, R110, R113, R123, R124, R125, R217, R218, R221, R222, R251, R253, R256, R258, R278, R280, R283, R285, R290, R291, R294, R295, R324, R326, R329, R331, R351, R353, R356, R358, R_EN2, R_EN4, R_EN6, R_EN8</t>
-  </si>
-  <si>
-    <t>R52, R58, R_EN1, R_EN3, R_EN5, R_EN7, R_FB1, R_FB5</t>
+    <t>R52, R69, R70, R71, R77, R78, R79, R85, R86, R87, R93, R94, R95, R101, R102, R103, R108, R112, R116, R120, R127, R128, R129, R223, R224, R227, R228, R257, R259, R262, R264, R284, R286, R289, R291, R296, R297, R300, R301, R330, R332, R335, R337, R357, R359, R362, R364, R_EN2, R_EN4, R_EN6, R_EN8</t>
+  </si>
+  <si>
+    <t>R56, R62, R_EN1, R_EN3, R_EN5, R_EN7</t>
   </si>
   <si>
     <t>100к</t>
   </si>
   <si>
-    <t>R55</t>
+    <t>R59, R_FB4, R_FB5</t>
   </si>
   <si>
     <t>12к</t>
   </si>
   <si>
-    <t>R56</t>
+    <t>R60</t>
   </si>
   <si>
     <t>110к</t>
   </si>
   <si>
-    <t>R57, R59, R206, R240, R243, R267, R270, R313, R316, R340, R343</t>
+    <t>R61, R63, R246, R249, R273, R276, R319, R322, R346, R349</t>
   </si>
   <si>
     <t>0</t>
   </si>
   <si>
-    <t>R61, R191, R199</t>
+    <t>R65, R197, R205</t>
   </si>
   <si>
     <t>20к</t>
   </si>
   <si>
-    <t>R62</t>
+    <t>R66</t>
   </si>
   <si>
     <t>61к</t>
   </si>
   <si>
-    <t>R63, R71, R79, R87, R95</t>
+    <t>R67, R75, R83, R91, R99</t>
   </si>
   <si>
     <t>10мОм 0.5% 100ppm/°C</t>
   </si>
   <si>
-    <t>R103, R106, R109, R112</t>
-  </si>
-  <si>
-    <t>R105, R108, R111, R114, R131, R135, R137, R139, R142, R145, R148, R151, R154, R157, R160, R163, R166, R169, R172, R175, R178, R181, R184, R201, R202, R238, R246, R249, R252, R260, R265, R273, R276, R279, R287, R311, R319, R322, R325, R333, R338, R346, R349, R352, R360</t>
+    <t>R107, R111, R115, R119</t>
+  </si>
+  <si>
+    <t>R109, R113, R117, R121</t>
+  </si>
+  <si>
+    <t>4.87к</t>
+  </si>
+  <si>
+    <t>R110, R114, R118, R122, R135, R139, R141, R143, R146, R149, R152, R155, R158, R161, R164, R167, R170, R173, R176, R179, R182, R185, R188, R207, R208, R244, R252, R255, R258, R266, R271, R279, R282, R285, R293, R317, R325, R328, R331, R339, R344, R352, R355, R358, R366</t>
   </si>
   <si>
     <t>10</t>
   </si>
   <si>
-    <t>R133, R136, R138, R143, R149, R155, R161, R167, R173, R179, R185</t>
-  </si>
-  <si>
-    <t>R140, R141, R146, R147, R152, R153, R158, R159, R164, R165, R170, R171, R176, R177, R182, R183, R261, R262, R288, R289, R334, R335, R361, R362</t>
+    <t>R137, R140, R142, R147, R153, R159, R165, R171, R177, R183, R189</t>
+  </si>
+  <si>
+    <t>R144, R145, R150, R151, R156, R157, R162, R163, R168, R169, R174, R175, R180, R181, R186, R187, R267, R268, R294, R295, R340, R341, R367, R368</t>
   </si>
   <si>
     <t>20</t>
   </si>
   <si>
-    <t>R192, R200</t>
+    <t>R198, R206</t>
   </si>
   <si>
     <t>470к</t>
   </si>
   <si>
-    <t>R193, R196, R204, R_FB6, R_FB8</t>
+    <t>R199, R202, R210</t>
   </si>
   <si>
     <t>47к</t>
   </si>
   <si>
-    <t>R195</t>
+    <t>R201</t>
   </si>
   <si>
     <t>5.6к</t>
   </si>
   <si>
-    <t>R197, R205</t>
+    <t>R203, R211</t>
   </si>
   <si>
     <t>1.6к</t>
   </si>
   <si>
-    <t>R225, R226, R237, R239, R242, R264, R266, R269, R298, R299, R310, R312, R315, R337, R339, R342</t>
+    <t>R231, R232, R243, R245, R248, R270, R272, R275, R304, R305, R316, R318, R321, R343, R345, R348</t>
   </si>
   <si>
     <t>49.9</t>
   </si>
   <si>
-    <t>R234, R307</t>
+    <t>R240, R313</t>
   </si>
   <si>
     <t>1500</t>
   </si>
   <si>
-    <t>R235, R308</t>
+    <t>R241, R314</t>
   </si>
   <si>
     <t>430</t>
   </si>
   <si>
-    <t>R_FB2</t>
-  </si>
-  <si>
-    <t>200к</t>
-  </si>
-  <si>
-    <t>R_FB3, R_FB7</t>
-  </si>
-  <si>
-    <t>150к</t>
-  </si>
-  <si>
-    <t>R_FB4</t>
-  </si>
-  <si>
-    <t>120к</t>
+    <t>R369, R370</t>
+  </si>
+  <si>
+    <t>4к7</t>
+  </si>
+  <si>
+    <t>R_FB1</t>
+  </si>
+  <si>
+    <t>7к5</t>
+  </si>
+  <si>
+    <t>R_FB2, R_FB3</t>
+  </si>
+  <si>
+    <t>15к</t>
+  </si>
+  <si>
+    <t>R_FB6</t>
+  </si>
+  <si>
+    <t>5к6</t>
+  </si>
+  <si>
+    <t>R_FB7</t>
+  </si>
+  <si>
+    <t>16к</t>
+  </si>
+  <si>
+    <t>R_FB8</t>
+  </si>
+  <si>
+    <t>5к1</t>
   </si>
   <si>
     <t>RJ1, RJ2</t>
@@ -637,7 +673,7 @@
     <t>ADT1-6T</t>
   </si>
   <si>
-    <t>TP1, TP2, TP3, TP4, TP5, TP6, TP7, TP8, TP9, TP10, TP11, TP12, TP13, TP14, TP15, TP16, TP17, TP18, TP19, TP20, TP21, TP22, TP23, TP24</t>
+    <t>TP1, TP2, TP3, TP4, TP5, TP6, TP7, TP8, TP9, TP10, TP11, TP12, TP13, TP14, TP15, TP16, TP17, TP18, TP19, TP20, TP21, TP22, TP23, TP24, TP25, TP26, TP27, TP28, TP29, TP30, TP31, TP32, TP33, TP34, TP35, TP36</t>
   </si>
   <si>
     <t>Контроль параметров платы</t>
@@ -664,16 +700,10 @@
     <t>U2</t>
   </si>
   <si>
-    <t>Intel® Cyclone® 10 LP FPGA</t>
-  </si>
-  <si>
-    <t>10CL016YU484С6</t>
-  </si>
-  <si>
-    <t>UBGA-484</t>
-  </si>
-  <si>
-    <t>U3</t>
+    <t>FBGA484_A-240</t>
+  </si>
+  <si>
+    <t>U4</t>
   </si>
   <si>
     <t xml:space="preserve">Precision Instrumentation Amplifier </t>
@@ -685,7 +715,7 @@
     <t>SOIC-8</t>
   </si>
   <si>
-    <t>U4</t>
+    <t>U5</t>
   </si>
   <si>
     <t>Аналоговый двухканальный мультиплексор</t>
@@ -697,7 +727,7 @@
     <t>TSSOP-16N</t>
   </si>
   <si>
-    <t>U5</t>
+    <t>U6</t>
   </si>
   <si>
     <t>18-Bit, 1.6Msps, Low Power SAR ADC with 101.2dB SNR</t>
@@ -709,7 +739,7 @@
     <t>MSOP16</t>
   </si>
   <si>
-    <t>U6</t>
+    <t>U7</t>
   </si>
   <si>
     <t>Single-Ended to Differential Converter/ADC Driver</t>
@@ -721,7 +751,7 @@
     <t>MSOP-8</t>
   </si>
   <si>
-    <t>U7</t>
+    <t>U8</t>
   </si>
   <si>
     <t>0.25ppm Noise, Low Drift Precision References</t>
@@ -730,7 +760,7 @@
     <t>LTC6655LNBHMS8-5</t>
   </si>
   <si>
-    <t>U8, U35, U38, U42, U45</t>
+    <t>U9, U40, U43, U47, U50</t>
   </si>
   <si>
     <t>Rail-to-Rail Input/Output Amplifiers, 3.1 nV/√Hz, 1 mA, 180 MHz</t>
@@ -742,7 +772,7 @@
     <t>SOT23-6</t>
   </si>
   <si>
-    <t>U9, U11</t>
+    <t>U10, U12</t>
   </si>
   <si>
     <t>20 V, 200 mA, Low Noise, CMOS LDO Linear Regulator</t>
@@ -754,7 +784,7 @@
     <t>TSOT-5</t>
   </si>
   <si>
-    <t>U10, U12</t>
+    <t>U11, U13</t>
   </si>
   <si>
     <t>–28 V, −200 mA, Low Noise, Linear Regulator</t>
@@ -763,7 +793,7 @@
     <t>ADP7182AUJZ-R7</t>
   </si>
   <si>
-    <t>U13, U14, U15, U16, U17</t>
+    <t>U14, U15, U16, U17, U18</t>
   </si>
   <si>
     <t>High-Side or Low-Side Measurement,</t>
@@ -775,7 +805,19 @@
     <t>VSSOP-10</t>
   </si>
   <si>
-    <t>U18, U19</t>
+    <t>U19, U20, U21, U22</t>
+  </si>
+  <si>
+    <t>Buck Converter</t>
+  </si>
+  <si>
+    <t>TPS62913RPUR</t>
+  </si>
+  <si>
+    <t>RPU0010A</t>
+  </si>
+  <si>
+    <t>U23, U24</t>
   </si>
   <si>
     <t>Датчик температуры I2C</t>
@@ -787,7 +829,7 @@
     <t>WSON-8</t>
   </si>
   <si>
-    <t>U20, U21, U22, U23, U24, U25, U26, U27, U28, U33, U37, U40, U44, U47</t>
+    <t>U25, U26, U27, U28, U29, U30, U31, U32, U33, U38, U42, U45, U49, U52</t>
   </si>
   <si>
     <t>TinyLogic UHS Triple Buffer</t>
@@ -799,7 +841,7 @@
     <t>US-8</t>
   </si>
   <si>
-    <t>U29</t>
+    <t>U34</t>
   </si>
   <si>
     <t>USB TO BASIC UART IC</t>
@@ -811,7 +853,7 @@
     <t>DFN-12</t>
   </si>
   <si>
-    <t>U30, U31</t>
+    <t>U35, U36</t>
   </si>
   <si>
     <t>2.7 - 23 V, 5.5 A, 28-mΩ True Reverse Current Blocking eFuse with Input</t>
@@ -823,7 +865,7 @@
     <t>VQFN-HR-10</t>
   </si>
   <si>
-    <t>U32</t>
+    <t>U37</t>
   </si>
   <si>
     <t>Programmable NOR flash memory</t>
@@ -835,7 +877,7 @@
     <t>WSON-8_6x8</t>
   </si>
   <si>
-    <t>U34, U41</t>
+    <t>U39, U46</t>
   </si>
   <si>
     <t>Dual 14-Bit Digital-to-Analog Converter, 250 Msps, -40 to +85 degC, CP-72-1, Pb-Free, Tray</t>
@@ -847,7 +889,7 @@
     <t>LFCSP-72</t>
   </si>
   <si>
-    <t>U36, U39, U43, U46</t>
+    <t>U41, U44, U48, U51</t>
   </si>
   <si>
     <t>Dual output clock buffer</t>
@@ -913,7 +955,7 @@
     <t>EPG.0B.302.HLN</t>
   </si>
   <si>
-    <t>X6, X7, X29, X31, X34, X36, X39, X41, X44, X46</t>
+    <t>X6, X7, X30, X32, X35, X37, X40, X42, X45, X47</t>
   </si>
   <si>
     <t>Jumper, 3-Pin, Dual row</t>
@@ -946,7 +988,7 @@
     <t>KLS1-4.20-2X04</t>
   </si>
   <si>
-    <t>X13, X14, X15, X16, X17, X18, X19, X20, X21, X30, X35, X40, X45</t>
+    <t>X13, X14, X15, X16, X17, X18, X19, X20, X21, X31, X36, X41, X46</t>
   </si>
   <si>
     <t>Jumper, 2-Pin, Dual row</t>
@@ -958,7 +1000,19 @@
     <t>PLS-2</t>
   </si>
   <si>
-    <t>X22</t>
+    <t>X22, X33, X34, X38, X39, X43, X44, X48, X49</t>
+  </si>
+  <si>
+    <t>Header, 4-Pin, Single row</t>
+  </si>
+  <si>
+    <t>Header 1X4</t>
+  </si>
+  <si>
+    <t>PLS-4</t>
+  </si>
+  <si>
+    <t>X23</t>
   </si>
   <si>
     <t>MicroUSB bottom mount receptacle, B-type</t>
@@ -970,7 +1024,7 @@
     <t>MicroUSB-Molex-105017</t>
   </si>
   <si>
-    <t>X23</t>
+    <t>X24</t>
   </si>
   <si>
     <t>Header, 10-Pin, Dual row</t>
@@ -979,22 +1033,10 @@
     <t>DS1013-10R</t>
   </si>
   <si>
-    <t>X24, X25, X26, X27, X28</t>
+    <t>X25, X26, X27, X28, X29</t>
   </si>
   <si>
     <t>PLD2-10</t>
-  </si>
-  <si>
-    <t>X32, X33, X37, X38, X42, X43, X47, X48</t>
-  </si>
-  <si>
-    <t>Header, 4-Pin, Single row</t>
-  </si>
-  <si>
-    <t>Header 1X4</t>
-  </si>
-  <si>
-    <t>PLS-4</t>
   </si>
   <si>
     <t>Y1</t>
@@ -1395,22 +1437,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E90A73E3-D209-4859-A4A1-8FA39F88837D}">
-  <dimension ref="A1:F116"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C5AF65-A1A3-40E0-954B-C21F5325B4CD}">
+  <dimension ref="A1:F123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="58" customWidth="1"/>
-    <col min="2" max="2" width="33.7109375" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="35.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="55.77734375" customWidth="1"/>
+    <col min="2" max="2" width="32.5546875" customWidth="1"/>
+    <col min="3" max="3" width="23.5546875" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="34.21875" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1430,7 +1472,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1450,7 +1492,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -1470,7 +1512,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -1490,7 +1532,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
@@ -1510,7 +1552,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
@@ -1530,7 +1572,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
@@ -1550,7 +1592,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
@@ -1570,7 +1612,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>27</v>
       </c>
@@ -1590,7 +1632,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>32</v>
       </c>
@@ -1610,7 +1652,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>35</v>
       </c>
@@ -1630,7 +1672,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>37</v>
       </c>
@@ -1650,7 +1692,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>39</v>
       </c>
@@ -1670,7 +1712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>42</v>
       </c>
@@ -1690,7 +1732,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>44</v>
       </c>
@@ -1710,7 +1752,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>46</v>
       </c>
@@ -1727,10 +1769,10 @@
         <v>12</v>
       </c>
       <c r="F16" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>48</v>
       </c>
@@ -1738,19 +1780,19 @@
         <v>7</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="E17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="1">
         <v>12</v>
       </c>
-      <c r="F17" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>50</v>
       </c>
@@ -1764,13 +1806,13 @@
         <v>51</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="F18" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
@@ -1787,10 +1829,10 @@
         <v>10</v>
       </c>
       <c r="F19" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>54</v>
       </c>
@@ -1798,19 +1840,19 @@
         <v>7</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F20" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>56</v>
       </c>
@@ -1824,13 +1866,13 @@
         <v>57</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F21" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>58</v>
       </c>
@@ -1844,13 +1886,13 @@
         <v>59</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F22" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>60</v>
       </c>
@@ -1867,10 +1909,10 @@
         <v>12</v>
       </c>
       <c r="F23" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>62</v>
       </c>
@@ -1887,10 +1929,10 @@
         <v>12</v>
       </c>
       <c r="F24" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>64</v>
       </c>
@@ -1907,10 +1949,10 @@
         <v>12</v>
       </c>
       <c r="F25" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>66</v>
       </c>
@@ -1927,10 +1969,10 @@
         <v>12</v>
       </c>
       <c r="F26" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>68</v>
       </c>
@@ -1947,202 +1989,204 @@
         <v>12</v>
       </c>
       <c r="F27" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="E28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="B29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F28" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D29" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F29" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F30" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="F31" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D31" s="1"/>
-      <c r="E31" s="2" t="s">
+      <c r="B32" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F31" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="E32" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F32" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="D32" s="1"/>
-      <c r="E32" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="F32" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F33" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F34" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F34" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="D35" s="1"/>
+      <c r="E35" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F35" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F35" s="1">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>97</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F36" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>97</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="F37" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>97</v>
@@ -2151,18 +2195,18 @@
         <v>98</v>
       </c>
       <c r="D38" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F38" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F38" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>109</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>97</v>
@@ -2171,18 +2215,18 @@
         <v>98</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>100</v>
       </c>
       <c r="F39" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>97</v>
@@ -2191,1463 +2235,1597 @@
         <v>98</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>100</v>
       </c>
       <c r="F40" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F41" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B41" s="2" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="B42" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="E42" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F42" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="B43" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F41" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D42" s="2" t="s">
+      <c r="C43" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="E43" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F43" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F42" s="1">
+      <c r="C44" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F44" s="1">
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F45" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F43" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E44" s="2" t="s">
+      <c r="F46" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F44" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F45" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F46" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="C47" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D47" s="2" t="s">
+      <c r="E47" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>133</v>
       </c>
       <c r="F47" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>123</v>
-      </c>
       <c r="E48" s="2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="F48" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>135</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D49" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F49" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="B50" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F49" s="1">
+      <c r="C50" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F50" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F51" s="1">
         <v>72</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E50" s="2" t="s">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F50" s="1">
+      <c r="C52" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F52" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E51" s="2" t="s">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F51" s="1">
+      <c r="C53" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F53" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="E52" s="2" t="s">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F52" s="1">
+      <c r="C54" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F54" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E53" s="2" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F53" s="1">
+      <c r="C55" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F55" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F54" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F55" s="1">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>148</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>149</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="F56" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>150</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D57" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F57" s="1">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="E57" s="2" t="s">
+      <c r="B58" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F57" s="1">
+      <c r="C58" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F58" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F59" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F60" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E58" s="2" t="s">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F58" s="1">
+      <c r="C61" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F61" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F62" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F63" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F59" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F60" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F61" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F62" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F63" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>163</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>164</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>117</v>
+        <v>132</v>
       </c>
       <c r="F64" s="1">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>165</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D65" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E65" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E65" s="2" t="s">
-        <v>117</v>
-      </c>
       <c r="F65" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>166</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>167</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="F66" s="1">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>168</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>169</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="F67" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>170</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D68" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F68" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="E68" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F68" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
+      <c r="C69" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D69" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B69" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D69" s="2" t="s">
+      <c r="E69" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F69" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="E69" s="2" t="s">
+      <c r="B70" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F69" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
+      <c r="C70" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D70" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B70" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>175</v>
-      </c>
       <c r="E70" s="2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="F70" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D71" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="B71" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D71" s="2" t="s">
+      <c r="E71" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F71" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="E71" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F71" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
+      <c r="C72" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D72" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B72" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D72" s="2" t="s">
+      <c r="E72" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F72" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="E72" s="2" t="s">
+      <c r="B73" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F72" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
+      <c r="C73" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D73" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="B73" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>181</v>
-      </c>
       <c r="E73" s="2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="F73" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D74" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="B74" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D74" s="2" t="s">
+      <c r="E74" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F74" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="E74" s="2" t="s">
+      <c r="B75" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F74" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
+      <c r="C75" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D75" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B75" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>185</v>
-      </c>
       <c r="E75" s="2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="F75" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D76" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B76" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D76" s="2" t="s">
+      <c r="E76" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F76" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E76" s="2" t="s">
+      <c r="B77" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F76" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
+      <c r="C77" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D77" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B77" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>155</v>
-      </c>
       <c r="E77" s="2" t="s">
-        <v>190</v>
+        <v>120</v>
       </c>
       <c r="F77" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F78" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B78" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F78" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
+      <c r="B79" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D79" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B79" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="E79" s="2" t="s">
-        <v>190</v>
+        <v>120</v>
       </c>
       <c r="F79" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>193</v>
       </c>
       <c r="B80" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D80" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="E80" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F80" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="D80" s="1"/>
-      <c r="E80" s="2" t="s">
+      <c r="B81" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D81" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="F80" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
+      <c r="E81" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F81" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B82" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D82" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="E82" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F82" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="D81" s="1"/>
-      <c r="E81" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="F81" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="s">
+      <c r="B83" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="C83" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E83" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="F83" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="D82" s="1"/>
-      <c r="E82" s="2" t="s">
+      <c r="B84" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F84" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="F82" s="1">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="2" t="s">
+      <c r="B85" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F85" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B86" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="C86" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="D83" s="1"/>
-      <c r="E83" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="F83" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="D84" s="1"/>
-      <c r="E84" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="F84" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="D85" s="1"/>
-      <c r="E85" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="F85" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>218</v>
       </c>
       <c r="D86" s="1"/>
       <c r="E86" s="2" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="F86" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="D87" s="1"/>
       <c r="E87" s="2" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="F87" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="D88" s="1"/>
       <c r="E88" s="2" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="F88" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="D89" s="1"/>
       <c r="E89" s="2" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="F89" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>233</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="B90" s="1"/>
+      <c r="C90" s="1"/>
       <c r="D90" s="1"/>
       <c r="E90" s="2" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="F90" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="D91" s="1"/>
       <c r="E91" s="2" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="F91" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="D92" s="1"/>
       <c r="E92" s="2" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="F92" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="D93" s="1"/>
       <c r="E93" s="2" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="F93" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="D94" s="1"/>
       <c r="E94" s="2" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="F94" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="D95" s="1"/>
       <c r="E95" s="2" t="s">
-        <v>253</v>
+        <v>236</v>
       </c>
       <c r="F95" s="1">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="D96" s="1"/>
       <c r="E96" s="2" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="F96" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="D97" s="1"/>
       <c r="E97" s="2" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
       <c r="F97" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="D98" s="1"/>
       <c r="E98" s="2" t="s">
-        <v>265</v>
+        <v>247</v>
       </c>
       <c r="F98" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="D99" s="1"/>
       <c r="E99" s="2" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="F99" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="D100" s="1"/>
       <c r="E100" s="2" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="F100" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="D101" s="1"/>
       <c r="E101" s="2" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="F101" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="D102" s="1"/>
       <c r="E102" s="2" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="F102" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="D103" s="1"/>
       <c r="E103" s="2" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="F103" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
       <c r="D104" s="1"/>
       <c r="E104" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="F104" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="D105" s="1"/>
       <c r="E105" s="2" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="F105" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="D106" s="1"/>
       <c r="E106" s="2" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="F106" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="D107" s="1"/>
       <c r="E107" s="2" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="F107" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="D108" s="1"/>
       <c r="E108" s="2" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="F108" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="D109" s="1"/>
       <c r="E109" s="2" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
       <c r="F109" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="D110" s="1"/>
       <c r="E110" s="2" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="F110" s="1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>308</v>
+        <v>288</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="D111" s="1"/>
       <c r="E111" s="2" t="s">
-        <v>310</v>
+        <v>290</v>
       </c>
       <c r="F111" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>312</v>
+        <v>300</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>313</v>
+        <v>301</v>
       </c>
       <c r="D112" s="1"/>
       <c r="E112" s="2" t="s">
-        <v>313</v>
+        <v>301</v>
       </c>
       <c r="F112" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
-        <v>314</v>
+        <v>302</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="D113" s="1"/>
       <c r="E113" s="2" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="F113" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
       <c r="D114" s="1"/>
       <c r="E114" s="2" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
       <c r="F114" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="D115" s="1"/>
       <c r="E115" s="2" t="s">
-        <v>323</v>
+        <v>311</v>
       </c>
       <c r="F115" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>326</v>
+        <v>314</v>
       </c>
       <c r="D116" s="1"/>
       <c r="E116" s="2" t="s">
-        <v>327</v>
+        <v>315</v>
       </c>
       <c r="F116" s="1">
         <v>1</v>
       </c>
     </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A117" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="D117" s="1"/>
+      <c r="E117" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="F117" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A118" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="D118" s="1"/>
+      <c r="E118" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="F118" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A119" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="D119" s="1"/>
+      <c r="E119" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="F119" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A120" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="D120" s="1"/>
+      <c r="E120" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F120" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A121" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="D121" s="1"/>
+      <c r="E121" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="F121" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A122" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="D122" s="1"/>
+      <c r="E122" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="F122" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A123" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="D123" s="1"/>
+      <c r="E123" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="F123" s="1">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>